<commit_message>
grafico de sistemas operativos
</commit_message>
<xml_diff>
--- a/src/assets/EQUIPOS.xlsx
+++ b/src/assets/EQUIPOS.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{9F0DFF40-5C1E-4995-B027-03C139BAD39C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8701A744-7870-4E87-8A8C-6C442C857104}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D43354-BA8D-4B6A-85EA-3BD1C82DFF42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventario Activo" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="521">
   <si>
     <t>Etiqueta</t>
   </si>
@@ -1365,12 +1365,6 @@
   </si>
   <si>
     <t>Windows 11</t>
-  </si>
-  <si>
-    <t>Windows  11</t>
-  </si>
-  <si>
-    <t>Windows  10</t>
   </si>
   <si>
     <t>Asistente de Almacen</t>
@@ -1590,7 +1584,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1622,6 +1616,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1643,7 +1645,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1664,6 +1666,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1687,10 +1692,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1754,17 +1759,17 @@
     <tableColumn id="1" xr3:uid="{59771C38-00B0-4DC3-A168-A8045865F88D}" name="Etiqueta" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{627A4378-150B-4A3C-A648-4A8C30C8FB4F}" name="Nombre Equipo" dataDxfId="12"/>
     <tableColumn id="13" xr3:uid="{675561B9-A7DF-4E72-81E3-008CAC8DFC93}" name="Descripcion" dataDxfId="11"/>
-    <tableColumn id="14" xr3:uid="{EDCD586D-3E75-40D3-AE2D-0C7C2421BBF7}" name="Sistema Operativo" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{7317A614-AF52-4445-8680-EDF4C44A4ED6}" name="Tipo" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{575E04CE-ADA7-4A46-9B38-0DEEC37BAAC4}" name="Marca" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{85DFE964-4E88-42FC-88D8-5C08E882C6DD}" name="Modelo" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{DE9894AB-9890-4C2F-9A0C-8783E65C14B5}" name="N° Serie" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{BCCEA834-3C77-4E06-9D8C-67999A34547B}" name="Responsable (Jefe)" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{71B53A87-5001-4030-AD35-BEE60073C474}" name="Perfiles Acceso" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{5CAF7C00-C970-4073-8691-F4347BC58C29}" name="Área" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{78DD8382-26BF-4C5C-8C57-534988D70E3A}" name="Departamento" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{B87B9A43-D1D7-4542-9F53-E0443B7A73AE}" name="Estado" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{DD0808EE-5530-4CB9-9BA6-C18B9161345D}" name="IP" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{EDCD586D-3E75-40D3-AE2D-0C7C2421BBF7}" name="Sistema Operativo" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{7317A614-AF52-4445-8680-EDF4C44A4ED6}" name="Tipo" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{575E04CE-ADA7-4A46-9B38-0DEEC37BAAC4}" name="Marca" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{85DFE964-4E88-42FC-88D8-5C08E882C6DD}" name="Modelo" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{DE9894AB-9890-4C2F-9A0C-8783E65C14B5}" name="N° Serie" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{BCCEA834-3C77-4E06-9D8C-67999A34547B}" name="Responsable (Jefe)" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{71B53A87-5001-4030-AD35-BEE60073C474}" name="Perfiles Acceso" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{5CAF7C00-C970-4073-8691-F4347BC58C29}" name="Área" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{78DD8382-26BF-4C5C-8C57-534988D70E3A}" name="Departamento" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{B87B9A43-D1D7-4542-9F53-E0443B7A73AE}" name="Estado" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{DD0808EE-5530-4CB9-9BA6-C18B9161345D}" name="IP" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2092,10 +2097,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N102"/>
+  <dimension ref="A1:N103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2235,7 +2240,7 @@
         <v>34</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>448</v>
@@ -2273,7 +2278,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>449</v>
@@ -2314,7 +2319,7 @@
         <v>39</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>449</v>
@@ -2352,7 +2357,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>449</v>
@@ -2390,7 +2395,7 @@
         <v>41</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>449</v>
@@ -2425,7 +2430,7 @@
         <v>42</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>449</v>
@@ -2463,7 +2468,7 @@
         <v>43</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>449</v>
@@ -2501,7 +2506,7 @@
         <v>44</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>449</v>
@@ -2539,7 +2544,7 @@
         <v>45</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>449</v>
@@ -2577,7 +2582,7 @@
         <v>46</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>449</v>
@@ -2682,7 +2687,7 @@
         <v>49</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>449</v>
@@ -2752,7 +2757,7 @@
         <v>51</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>449</v>
@@ -2790,7 +2795,7 @@
         <v>52</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>447</v>
@@ -2928,7 +2933,7 @@
         <v>56</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>449</v>
@@ -2963,7 +2968,7 @@
         <v>57</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>449</v>
@@ -3001,7 +3006,7 @@
         <v>58</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>449</v>
@@ -3039,7 +3044,7 @@
         <v>59</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>449</v>
@@ -3077,7 +3082,7 @@
         <v>60</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>449</v>
@@ -3115,7 +3120,7 @@
         <v>61</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>449</v>
@@ -3153,7 +3158,7 @@
         <v>62</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>449</v>
@@ -3191,7 +3196,7 @@
         <v>63</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>449</v>
@@ -3229,7 +3234,7 @@
         <v>64</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>449</v>
@@ -3267,7 +3272,7 @@
         <v>65</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>447</v>
@@ -3305,7 +3310,7 @@
         <v>66</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>449</v>
@@ -3340,7 +3345,7 @@
         <v>67</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>447</v>
@@ -3378,7 +3383,7 @@
         <v>68</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>447</v>
@@ -3416,7 +3421,7 @@
         <v>69</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>449</v>
@@ -3454,7 +3459,7 @@
         <v>70</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>449</v>
@@ -3492,7 +3497,7 @@
         <v>71</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>449</v>
@@ -3530,7 +3535,7 @@
         <v>72</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>449</v>
@@ -3632,7 +3637,7 @@
         <v>75</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>449</v>
@@ -3705,7 +3710,7 @@
         <v>77</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>449</v>
@@ -3743,7 +3748,7 @@
         <v>78</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>449</v>
@@ -3851,7 +3856,7 @@
         <v>81</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>449</v>
@@ -3889,7 +3894,7 @@
         <v>82</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>449</v>
@@ -3927,7 +3932,7 @@
         <v>83</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>449</v>
@@ -3965,7 +3970,7 @@
         <v>84</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>449</v>
@@ -4035,7 +4040,7 @@
         <v>86</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>449</v>
@@ -4073,7 +4078,7 @@
         <v>87</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>449</v>
@@ -4111,7 +4116,7 @@
         <v>88</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>449</v>
@@ -4149,7 +4154,7 @@
         <v>89</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>449</v>
@@ -4187,7 +4192,7 @@
         <v>90</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>449</v>
@@ -4225,7 +4230,7 @@
         <v>91</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>449</v>
@@ -4263,7 +4268,7 @@
         <v>92</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>449</v>
@@ -4301,7 +4306,7 @@
         <v>93</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>449</v>
@@ -4339,7 +4344,7 @@
         <v>94</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>449</v>
@@ -4377,7 +4382,7 @@
         <v>95</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>447</v>
@@ -4415,7 +4420,7 @@
         <v>96</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>449</v>
@@ -4453,7 +4458,7 @@
         <v>97</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>449</v>
@@ -4491,7 +4496,7 @@
         <v>98</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>447</v>
@@ -4529,7 +4534,7 @@
         <v>99</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>449</v>
@@ -4567,7 +4572,7 @@
         <v>100</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>449</v>
@@ -4605,7 +4610,7 @@
         <v>101</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>449</v>
@@ -4643,7 +4648,7 @@
         <v>102</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>449</v>
@@ -4681,7 +4686,7 @@
         <v>103</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>449</v>
@@ -4719,7 +4724,7 @@
         <v>104</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>449</v>
@@ -4912,7 +4917,7 @@
         <v>110</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>449</v>
@@ -4947,7 +4952,7 @@
         <v>111</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>449</v>
@@ -4982,7 +4987,7 @@
         <v>112</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>449</v>
@@ -5020,7 +5025,7 @@
         <v>113</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>449</v>
@@ -5096,7 +5101,7 @@
         <v>115</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>449</v>
@@ -5134,7 +5139,7 @@
         <v>116</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>449</v>
@@ -5207,7 +5212,7 @@
         <v>118</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>449</v>
@@ -5242,7 +5247,7 @@
         <v>119</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>449</v>
@@ -5280,7 +5285,7 @@
         <v>120</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>449</v>
@@ -5318,7 +5323,7 @@
         <v>121</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>449</v>
@@ -5356,7 +5361,7 @@
         <v>122</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>449</v>
@@ -5391,7 +5396,7 @@
         <v>123</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>449</v>
@@ -5490,7 +5495,7 @@
         <v>126</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>449</v>
@@ -5525,7 +5530,7 @@
         <v>127</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>449</v>
@@ -5560,7 +5565,7 @@
         <v>128</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>449</v>
@@ -5691,7 +5696,7 @@
         <v>132</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>449</v>
@@ -5726,7 +5731,7 @@
         <v>133</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>448</v>
@@ -5762,10 +5767,10 @@
         <v>358</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>134</v>
@@ -5797,7 +5802,7 @@
         <v>440</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>134</v>
@@ -5823,6 +5828,9 @@
       <c r="N102" s="5" t="s">
         <v>441</v>
       </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D103" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
nuevo widget de panda
</commit_message>
<xml_diff>
--- a/src/assets/EQUIPOS.xlsx
+++ b/src/assets/EQUIPOS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5BAB8D9-C387-420B-B8B4-17663652863E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A79754-4E62-46C8-81C6-C1E3D63D7E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1556" uniqueCount="637">
   <si>
     <t>Etiqueta</t>
   </si>
@@ -1814,21 +1814,6 @@
     <t>CROWNCUN\contador</t>
   </si>
   <si>
-    <t>Widows 11</t>
-  </si>
-  <si>
-    <t>Widows 10</t>
-  </si>
-  <si>
-    <t>Widows 7</t>
-  </si>
-  <si>
-    <t>Widows Server</t>
-  </si>
-  <si>
-    <t>Widows XP</t>
-  </si>
-  <si>
     <t>ARRIVA\aydcun01</t>
   </si>
   <si>
@@ -1917,6 +1902,30 @@
   </si>
   <si>
     <t>Office Hogar y Pequeña Empresa 2010</t>
+  </si>
+  <si>
+    <t>Windows 11</t>
+  </si>
+  <si>
+    <t>Windows 10</t>
+  </si>
+  <si>
+    <t>Windows 7</t>
+  </si>
+  <si>
+    <t>Windows Server</t>
+  </si>
+  <si>
+    <t>Windows XP</t>
+  </si>
+  <si>
+    <t>Panda</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -2016,7 +2025,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2042,19 +2051,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2065,7 +2065,7 @@
     <cellStyle name="60% - Énfasis4" xfId="1" builtinId="44"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="23">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2082,7 +2082,13 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2115,10 +2121,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2161,32 +2164,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EF8ACE9A-3DC4-4577-9E29-4CEAA3B671E9}" name="Tabla1" displayName="Tabla1" ref="A1:T102" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:T102" xr:uid="{EF8ACE9A-3DC4-4577-9E29-4CEAA3B671E9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EF8ACE9A-3DC4-4577-9E29-4CEAA3B671E9}" name="Tabla1" displayName="Tabla1" ref="A1:U102" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A1:U102" xr:uid="{EF8ACE9A-3DC4-4577-9E29-4CEAA3B671E9}">
+    <filterColumn colId="20">
+      <filters>
+        <filter val="X"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T102">
     <sortCondition ref="M1:M102"/>
   </sortState>
-  <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{59771C38-00B0-4DC3-A168-A8045865F88D}" name="Etiqueta" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{627A4378-150B-4A3C-A648-4A8C30C8FB4F}" name="Nombre Equipo" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{675561B9-A7DF-4E72-81E3-008CAC8DFC93}" name="Descripcion" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{EDCD586D-3E75-40D3-AE2D-0C7C2421BBF7}" name="Sistema Operativo" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{7317A614-AF52-4445-8680-EDF4C44A4ED6}" name="Tipo" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{575E04CE-ADA7-4A46-9B38-0DEEC37BAAC4}" name="Marca" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{85DFE964-4E88-42FC-88D8-5C08E882C6DD}" name="Modelo" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{DE9894AB-9890-4C2F-9A0C-8783E65C14B5}" name="N° Serie" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{BCCEA834-3C77-4E06-9D8C-67999A34547B}" name="Responsable (Jefe)" dataDxfId="10"/>
-    <tableColumn id="15" xr3:uid="{99BCC5ED-6FF5-4E38-911C-3D1511CA4A3F}" name="Usuario" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{71B53A87-5001-4030-AD35-BEE60073C474}" name="Perfiles Acceso" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{5CAF7C00-C970-4073-8691-F4347BC58C29}" name="Área" dataDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{78DD8382-26BF-4C5C-8C57-534988D70E3A}" name="Departamento" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{B87B9A43-D1D7-4542-9F53-E0443B7A73AE}" name="Estado" dataDxfId="12"/>
-    <tableColumn id="12" xr3:uid="{DD0808EE-5530-4CB9-9BA6-C18B9161345D}" name="IP" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{2BC6E608-CFAC-47A4-8753-08E722FD475E}" name="Version Office" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{EC074AD3-7E91-4532-9428-25FD0E397CC5}" name="Tipo Licencia" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{07F445C3-C102-40EF-A3D5-A2F375AAABAF}" name="N Producto" dataDxfId="2"/>
-    <tableColumn id="19" xr3:uid="{9D513EC3-19AE-46A1-9420-912FD802C1C6}" name="Inicio Garantia" dataDxfId="1"/>
-    <tableColumn id="20" xr3:uid="{174712AC-E5F0-410E-AD51-803D0A80E0E4}" name="Fin Garantia" dataDxfId="0"/>
+  <tableColumns count="21">
+    <tableColumn id="1" xr3:uid="{59771C38-00B0-4DC3-A168-A8045865F88D}" name="Etiqueta" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{627A4378-150B-4A3C-A648-4A8C30C8FB4F}" name="Nombre Equipo" dataDxfId="19"/>
+    <tableColumn id="13" xr3:uid="{675561B9-A7DF-4E72-81E3-008CAC8DFC93}" name="Descripcion" dataDxfId="18"/>
+    <tableColumn id="14" xr3:uid="{EDCD586D-3E75-40D3-AE2D-0C7C2421BBF7}" name="Sistema Operativo" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{7317A614-AF52-4445-8680-EDF4C44A4ED6}" name="Tipo" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{575E04CE-ADA7-4A46-9B38-0DEEC37BAAC4}" name="Marca" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{85DFE964-4E88-42FC-88D8-5C08E882C6DD}" name="Modelo" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{DE9894AB-9890-4C2F-9A0C-8783E65C14B5}" name="N° Serie" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{BCCEA834-3C77-4E06-9D8C-67999A34547B}" name="Responsable (Jefe)" dataDxfId="12"/>
+    <tableColumn id="15" xr3:uid="{99BCC5ED-6FF5-4E38-911C-3D1511CA4A3F}" name="Usuario" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{71B53A87-5001-4030-AD35-BEE60073C474}" name="Perfiles Acceso" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{5CAF7C00-C970-4073-8691-F4347BC58C29}" name="Área" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{78DD8382-26BF-4C5C-8C57-534988D70E3A}" name="Departamento" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{B87B9A43-D1D7-4542-9F53-E0443B7A73AE}" name="Estado" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{DD0808EE-5530-4CB9-9BA6-C18B9161345D}" name="IP" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{2BC6E608-CFAC-47A4-8753-08E722FD475E}" name="Version Office" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{EC074AD3-7E91-4532-9428-25FD0E397CC5}" name="Tipo Licencia" dataDxfId="4"/>
+    <tableColumn id="18" xr3:uid="{07F445C3-C102-40EF-A3D5-A2F375AAABAF}" name="N Producto" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{9D513EC3-19AE-46A1-9420-912FD802C1C6}" name="Inicio Garantia" dataDxfId="2"/>
+    <tableColumn id="20" xr3:uid="{174712AC-E5F0-410E-AD51-803D0A80E0E4}" name="Fin Garantia" dataDxfId="1"/>
+    <tableColumn id="21" xr3:uid="{429B1595-8D6F-40ED-86DE-82DD436792A5}" name="Panda" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2514,10 +2524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T103"/>
+  <dimension ref="A1:X104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="W89" sqref="W89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2541,10 +2551,11 @@
     <col min="18" max="18" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="3"/>
+    <col min="21" max="21" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2554,7 +2565,7 @@
       <c r="C1" s="7" t="s">
         <v>426</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="3" t="s">
         <v>427</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -2591,22 +2602,25 @@
         <v>11</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+        <v>621</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>338</v>
       </c>
@@ -2617,7 +2631,7 @@
         <v>437</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>14</v>
@@ -2647,13 +2661,16 @@
         <v>141</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>344</v>
       </c>
@@ -2664,7 +2681,7 @@
         <v>507</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>600</v>
+        <v>630</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>14</v>
@@ -2694,13 +2711,16 @@
         <v>142</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>47</v>
       </c>
@@ -2708,7 +2728,7 @@
         <v>514</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>14</v>
@@ -2738,13 +2758,16 @@
         <v>143</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>345</v>
       </c>
@@ -2755,7 +2778,7 @@
         <v>438</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>133</v>
@@ -2785,13 +2808,16 @@
         <v>144</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>347</v>
       </c>
@@ -2802,7 +2828,7 @@
         <v>511</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>14</v>
@@ -2832,13 +2858,16 @@
         <v>145</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>50</v>
       </c>
@@ -2846,7 +2875,7 @@
         <v>439</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>14</v>
@@ -2876,13 +2905,16 @@
         <v>146</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>348</v>
       </c>
@@ -2893,7 +2925,7 @@
         <v>440</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>14</v>
@@ -2920,8 +2952,11 @@
         <v>20</v>
       </c>
       <c r="O8"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U8" s="3" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>349</v>
       </c>
@@ -2932,7 +2967,7 @@
         <v>516</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>14</v>
@@ -2947,7 +2982,7 @@
         <v>226</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>312</v>
@@ -2961,14 +2996,17 @@
       <c r="O9" t="s">
         <v>147</v>
       </c>
-      <c r="P9" s="13" t="s">
-        <v>629</v>
+      <c r="P9" s="10" t="s">
+        <v>624</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>350</v>
       </c>
@@ -2979,7 +3017,7 @@
         <v>517</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>133</v>
@@ -2994,7 +3032,7 @@
         <v>227</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>312</v>
@@ -3008,14 +3046,17 @@
       <c r="O10" t="s">
         <v>148</v>
       </c>
-      <c r="P10" s="13" t="s">
-        <v>630</v>
+      <c r="P10" s="10" t="s">
+        <v>625</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>352</v>
       </c>
@@ -3026,7 +3067,7 @@
         <v>518</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>14</v>
@@ -3056,13 +3097,16 @@
         <v>149</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>55</v>
       </c>
@@ -3070,7 +3114,7 @@
         <v>441</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>133</v>
@@ -3084,7 +3128,7 @@
       <c r="H12" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="J12" s="1" t="s">
         <v>520</v>
       </c>
       <c r="L12" s="3" t="s">
@@ -3100,13 +3144,16 @@
         <v>150</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>356</v>
       </c>
@@ -3117,7 +3164,7 @@
         <v>445</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>14</v>
@@ -3146,8 +3193,11 @@
       <c r="O13" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>357</v>
       </c>
@@ -3158,7 +3208,7 @@
         <v>446</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>14</v>
@@ -3188,13 +3238,16 @@
         <v>153</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>358</v>
       </c>
@@ -3205,7 +3258,7 @@
         <v>447</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>600</v>
+        <v>630</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>133</v>
@@ -3235,13 +3288,16 @@
         <v>154</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>359</v>
       </c>
@@ -3252,7 +3308,7 @@
         <v>526</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>133</v>
@@ -3280,13 +3336,16 @@
       </c>
       <c r="O16"/>
       <c r="P16" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>360</v>
       </c>
@@ -3297,7 +3356,7 @@
         <v>448</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>133</v>
@@ -3311,7 +3370,7 @@
       <c r="H17" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J17" s="11" t="s">
+      <c r="J17" s="1" t="s">
         <v>528</v>
       </c>
       <c r="L17" s="3" t="s">
@@ -3324,16 +3383,19 @@
         <v>20</v>
       </c>
       <c r="O17" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U17" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>362</v>
       </c>
@@ -3344,7 +3406,7 @@
         <v>449</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>600</v>
+        <v>630</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>14</v>
@@ -3374,13 +3436,16 @@
         <v>155</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
@@ -3391,7 +3456,7 @@
         <v>428</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>14</v>
@@ -3405,7 +3470,7 @@
       <c r="H19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="10" t="s">
+      <c r="J19" s="9" t="s">
         <v>499</v>
       </c>
       <c r="L19" s="3" t="s">
@@ -3421,13 +3486,16 @@
         <v>21</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U19" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>330</v>
       </c>
@@ -3438,7 +3506,7 @@
         <v>429</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>14</v>
@@ -3468,13 +3536,16 @@
         <v>134</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>332</v>
       </c>
@@ -3485,7 +3556,7 @@
         <v>430</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>14</v>
@@ -3515,13 +3586,16 @@
         <v>135</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q21" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U21" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>354</v>
       </c>
@@ -3532,7 +3606,7 @@
         <v>443</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>133</v>
@@ -3562,13 +3636,16 @@
         <v>151</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>369</v>
       </c>
@@ -3579,7 +3656,7 @@
         <v>454</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>14</v>
@@ -3609,13 +3686,16 @@
         <v>161</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U23" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>370</v>
       </c>
@@ -3626,7 +3706,7 @@
         <v>454</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>14</v>
@@ -3656,13 +3736,16 @@
         <v>162</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U24" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>371</v>
       </c>
@@ -3673,7 +3756,7 @@
         <v>444</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>14</v>
@@ -3703,13 +3786,16 @@
         <v>163</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U25" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>72</v>
       </c>
@@ -3717,7 +3803,7 @@
         <v>548</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>133</v>
@@ -3745,13 +3831,16 @@
       </c>
       <c r="O26"/>
       <c r="P26" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q26" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U26" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>373</v>
       </c>
@@ -3762,7 +3851,7 @@
         <v>542</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>14</v>
@@ -3792,13 +3881,16 @@
         <v>164</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q27" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U27" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>74</v>
       </c>
@@ -3806,7 +3898,7 @@
         <v>455</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>14</v>
@@ -3836,13 +3928,16 @@
         <v>165</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q28" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U28" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>374</v>
       </c>
@@ -3851,7 +3946,7 @@
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>14</v>
@@ -3876,8 +3971,11 @@
         <v>20</v>
       </c>
       <c r="O29"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U29" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>375</v>
       </c>
@@ -3888,7 +3986,7 @@
         <v>456</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>133</v>
@@ -3915,16 +4013,19 @@
         <v>20</v>
       </c>
       <c r="O30" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q30" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U30" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>376</v>
       </c>
@@ -3935,7 +4036,7 @@
         <v>457</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>133</v>
@@ -3965,13 +4066,16 @@
         <v>166</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U31" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>377</v>
       </c>
@@ -3982,7 +4086,7 @@
         <v>540</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>14</v>
@@ -4012,13 +4116,16 @@
         <v>167</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q32" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U32" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>378</v>
       </c>
@@ -4027,7 +4134,7 @@
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>14</v>
@@ -4057,13 +4164,16 @@
         <v>168</v>
       </c>
       <c r="P33" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q33" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U33" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>379</v>
       </c>
@@ -4074,7 +4184,7 @@
         <v>458</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>14</v>
@@ -4104,13 +4214,16 @@
         <v>169</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q34" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U34" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>383</v>
       </c>
@@ -4121,7 +4234,7 @@
         <v>462</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>14</v>
@@ -4151,13 +4264,16 @@
         <v>173</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q35" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U35" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>384</v>
       </c>
@@ -4168,7 +4284,7 @@
         <v>463</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>14</v>
@@ -4198,13 +4314,16 @@
         <v>174</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q36" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U36" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>392</v>
       </c>
@@ -4215,7 +4334,7 @@
         <v>470</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>14</v>
@@ -4245,13 +4364,16 @@
         <v>181</v>
       </c>
       <c r="P37" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q37" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U37" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>110</v>
       </c>
@@ -4259,7 +4381,7 @@
         <v>481</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>14</v>
@@ -4289,13 +4411,16 @@
         <v>195</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q38" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U38" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
         <v>111</v>
       </c>
@@ -4303,7 +4428,7 @@
         <v>481</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>133</v>
@@ -4331,13 +4456,16 @@
       </c>
       <c r="O39"/>
       <c r="P39" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q39" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U39" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>408</v>
       </c>
@@ -4348,7 +4476,7 @@
         <v>482</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>133</v>
@@ -4375,16 +4503,19 @@
         <v>20</v>
       </c>
       <c r="O40" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="P40" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q40" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U40" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>342</v>
       </c>
@@ -4395,7 +4526,7 @@
         <v>496</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>133</v>
@@ -4425,19 +4556,22 @@
         <v>341</v>
       </c>
       <c r="P41" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q41" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U41" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
         <v>421</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>133</v>
@@ -4465,13 +4599,16 @@
         <v>422</v>
       </c>
       <c r="P42" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q42" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U42" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>333</v>
       </c>
@@ -4482,7 +4619,7 @@
         <v>431</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>14</v>
@@ -4512,13 +4649,16 @@
         <v>136</v>
       </c>
       <c r="P43" s="3" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="Q43" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+      <c r="U43" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>41</v>
       </c>
@@ -4526,7 +4666,7 @@
         <v>432</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>14</v>
@@ -4556,13 +4696,16 @@
         <v>137</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q44" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U44" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>334</v>
       </c>
@@ -4573,7 +4716,7 @@
         <v>433</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>14</v>
@@ -4603,13 +4746,16 @@
         <v>138</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q45" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U45" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>335</v>
       </c>
@@ -4620,7 +4766,7 @@
         <v>434</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>14</v>
@@ -4650,13 +4796,16 @@
         <v>139</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q46" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U46" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>363</v>
       </c>
@@ -4667,7 +4816,7 @@
         <v>450</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>14</v>
@@ -4697,13 +4846,16 @@
         <v>156</v>
       </c>
       <c r="P47" s="3" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="Q47" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+      <c r="U47" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>364</v>
       </c>
@@ -4714,7 +4866,7 @@
         <v>451</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>14</v>
@@ -4744,13 +4896,16 @@
         <v>157</v>
       </c>
       <c r="P48" s="3" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="Q48" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+      <c r="U48" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
         <v>66</v>
       </c>
@@ -4758,7 +4913,7 @@
         <v>533</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>14</v>
@@ -4788,13 +4943,16 @@
         <v>158</v>
       </c>
       <c r="P49" s="3" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="Q49" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+      <c r="U49" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>366</v>
       </c>
@@ -4805,7 +4963,7 @@
         <v>452</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>600</v>
+        <v>630</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>14</v>
@@ -4835,13 +4993,16 @@
         <v>159</v>
       </c>
       <c r="P50" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q50" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U50" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>368</v>
       </c>
@@ -4852,7 +5013,7 @@
         <v>453</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>14</v>
@@ -4882,13 +5043,16 @@
         <v>160</v>
       </c>
       <c r="P51" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q51" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U51" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>380</v>
       </c>
@@ -4899,7 +5063,7 @@
         <v>459</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>133</v>
@@ -4929,13 +5093,16 @@
         <v>170</v>
       </c>
       <c r="P52" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q52" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U52" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>385</v>
       </c>
@@ -4946,7 +5113,7 @@
         <v>464</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>14</v>
@@ -4976,13 +5143,16 @@
         <v>175</v>
       </c>
       <c r="P53" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q53" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U53" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>393</v>
       </c>
@@ -4993,7 +5163,7 @@
         <v>476</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>600</v>
+        <v>630</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>14</v>
@@ -5023,13 +5193,16 @@
         <v>182</v>
       </c>
       <c r="P54" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q54" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U54" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>394</v>
       </c>
@@ -5040,7 +5213,7 @@
         <v>474</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>14</v>
@@ -5070,13 +5243,16 @@
         <v>183</v>
       </c>
       <c r="P55" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q55" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U55" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>395</v>
       </c>
@@ -5087,7 +5263,7 @@
         <v>475</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>14</v>
@@ -5117,13 +5293,16 @@
         <v>184</v>
       </c>
       <c r="P56" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q56" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U56" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>396</v>
       </c>
@@ -5134,7 +5313,7 @@
         <v>473</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>600</v>
+        <v>630</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>14</v>
@@ -5164,13 +5343,16 @@
         <v>185</v>
       </c>
       <c r="P57" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q57" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U57" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>397</v>
       </c>
@@ -5181,7 +5363,7 @@
         <v>472</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>14</v>
@@ -5211,13 +5393,16 @@
         <v>186</v>
       </c>
       <c r="P58" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q58" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U58" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>398</v>
       </c>
@@ -5228,7 +5413,7 @@
         <v>471</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>14</v>
@@ -5258,13 +5443,16 @@
         <v>187</v>
       </c>
       <c r="P59" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q59" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U59" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>399</v>
       </c>
@@ -5275,7 +5463,7 @@
         <v>477</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>14</v>
@@ -5305,13 +5493,16 @@
         <v>188</v>
       </c>
       <c r="P60" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q60" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U60" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
         <v>104</v>
       </c>
@@ -5319,7 +5510,7 @@
         <v>573</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>14</v>
@@ -5347,13 +5538,16 @@
         <v>192</v>
       </c>
       <c r="P61" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q61" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U61" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>405</v>
       </c>
@@ -5364,7 +5558,7 @@
         <v>575</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>133</v>
@@ -5391,8 +5585,11 @@
         <v>20</v>
       </c>
       <c r="O62"/>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U62" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
         <v>106</v>
       </c>
@@ -5400,7 +5597,7 @@
         <v>576</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>133</v>
@@ -5427,8 +5624,11 @@
         <v>20</v>
       </c>
       <c r="O63"/>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U63" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
         <v>107</v>
       </c>
@@ -5436,7 +5636,7 @@
         <v>578</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>14</v>
@@ -5460,8 +5660,11 @@
       <c r="O64" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U64" s="3" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
         <v>108</v>
       </c>
@@ -5469,7 +5672,7 @@
         <v>580</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>14</v>
@@ -5498,8 +5701,11 @@
       <c r="O65" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U65" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
         <v>109</v>
       </c>
@@ -5507,7 +5713,7 @@
         <v>480</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>14</v>
@@ -5534,16 +5740,19 @@
         <v>20</v>
       </c>
       <c r="O66" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="P66" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q66" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U66" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>414</v>
       </c>
@@ -5554,7 +5763,7 @@
         <v>487</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>600</v>
+        <v>630</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>14</v>
@@ -5584,13 +5793,16 @@
         <v>201</v>
       </c>
       <c r="P67" s="3" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="Q67" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+      <c r="U67" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>417</v>
       </c>
@@ -5601,7 +5813,7 @@
         <v>488</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>600</v>
+        <v>630</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>14</v>
@@ -5631,13 +5843,16 @@
         <v>202</v>
       </c>
       <c r="P68" s="3" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="Q68" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+      <c r="U68" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>381</v>
       </c>
@@ -5648,7 +5863,7 @@
         <v>460</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>133</v>
@@ -5678,19 +5893,22 @@
         <v>171</v>
       </c>
       <c r="P69" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q69" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U69" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
         <v>84</v>
       </c>
       <c r="C70" s="4"/>
       <c r="D70" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>133</v>
@@ -5705,7 +5923,7 @@
         <v>258</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="L70" s="3" t="s">
         <v>322</v>
@@ -5720,19 +5938,22 @@
         <v>172</v>
       </c>
       <c r="P70" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q70" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U70" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C71" s="4"/>
       <c r="D71" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>133</v>
@@ -5747,7 +5968,7 @@
         <v>296</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="L71" s="3" t="s">
         <v>322</v>
@@ -5759,16 +5980,19 @@
         <v>20</v>
       </c>
       <c r="O71" t="s">
-        <v>617</v>
-      </c>
-      <c r="P71" s="14" t="s">
-        <v>629</v>
+        <v>612</v>
+      </c>
+      <c r="P71" s="11" t="s">
+        <v>624</v>
       </c>
       <c r="Q71" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+      <c r="U71" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
         <v>124</v>
       </c>
@@ -5776,7 +6000,7 @@
         <v>592</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>14</v>
@@ -5791,7 +6015,7 @@
         <v>297</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="L72" s="3" t="s">
         <v>322</v>
@@ -5806,13 +6030,16 @@
         <v>204</v>
       </c>
       <c r="P72" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q72" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U72" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
         <v>125</v>
       </c>
@@ -5820,7 +6047,7 @@
         <v>491</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>133</v>
@@ -5835,7 +6062,7 @@
         <v>298</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="L73" s="3" t="s">
         <v>322</v>
@@ -5850,13 +6077,16 @@
         <v>205</v>
       </c>
       <c r="P73" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q73" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U73" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
         <v>126</v>
       </c>
@@ -5864,7 +6094,7 @@
         <v>492</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>133</v>
@@ -5879,7 +6109,7 @@
         <v>299</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="L74" s="3" t="s">
         <v>322</v>
@@ -5894,13 +6124,16 @@
         <v>206</v>
       </c>
       <c r="P74" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q74" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U74" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
         <v>127</v>
       </c>
@@ -5908,7 +6141,7 @@
         <v>493</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>14</v>
@@ -5936,13 +6169,16 @@
       </c>
       <c r="O75"/>
       <c r="P75" s="3" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="Q75" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+      <c r="U75" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
         <v>128</v>
       </c>
@@ -5950,7 +6186,7 @@
         <v>594</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>14</v>
@@ -5965,7 +6201,7 @@
         <v>301</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="L76" s="3" t="s">
         <v>322</v>
@@ -5980,13 +6216,16 @@
         <v>207</v>
       </c>
       <c r="P76" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q76" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U76" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="s">
         <v>129</v>
       </c>
@@ -5994,7 +6233,7 @@
         <v>596</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>600</v>
+        <v>630</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>14</v>
@@ -6009,7 +6248,7 @@
         <v>302</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="L77" s="3" t="s">
         <v>322</v>
@@ -6021,8 +6260,11 @@
         <v>20</v>
       </c>
       <c r="O77"/>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U77" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
         <v>130</v>
       </c>
@@ -6030,7 +6272,7 @@
         <v>597</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>600</v>
+        <v>630</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>133</v>
@@ -6045,7 +6287,7 @@
         <v>303</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="L78" s="3" t="s">
         <v>322</v>
@@ -6060,13 +6302,16 @@
         <v>208</v>
       </c>
       <c r="P78" s="3" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="Q78" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+      <c r="U78" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
         <v>131</v>
       </c>
@@ -6074,7 +6319,7 @@
         <v>494</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>600</v>
+        <v>630</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>14</v>
@@ -6088,7 +6333,7 @@
       <c r="H79" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="J79" s="12" t="s">
+      <c r="J79" s="3" t="s">
         <v>595</v>
       </c>
       <c r="L79" s="3" t="s">
@@ -6104,13 +6349,16 @@
         <v>209</v>
       </c>
       <c r="P79" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q79" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U79" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>387</v>
       </c>
@@ -6121,7 +6369,7 @@
         <v>465</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>14</v>
@@ -6151,13 +6399,16 @@
         <v>176</v>
       </c>
       <c r="P80" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q80" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U80" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>388</v>
       </c>
@@ -6168,7 +6419,7 @@
         <v>466</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>14</v>
@@ -6182,7 +6433,7 @@
       <c r="H81" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="J81" s="10" t="s">
+      <c r="J81" s="9" t="s">
         <v>558</v>
       </c>
       <c r="L81" s="3" t="s">
@@ -6198,13 +6449,16 @@
         <v>177</v>
       </c>
       <c r="P81" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q81" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U81" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>389</v>
       </c>
@@ -6215,7 +6469,7 @@
         <v>467</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>14</v>
@@ -6229,7 +6483,7 @@
       <c r="H82" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="J82" s="10" t="s">
+      <c r="J82" s="9" t="s">
         <v>559</v>
       </c>
       <c r="L82" s="3" t="s">
@@ -6245,13 +6499,16 @@
         <v>178</v>
       </c>
       <c r="P82" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q82" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U82" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="83" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>390</v>
       </c>
@@ -6262,7 +6519,7 @@
         <v>468</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>133</v>
@@ -6276,7 +6533,7 @@
       <c r="H83" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="J83" s="10" t="s">
+      <c r="J83" s="9" t="s">
         <v>560</v>
       </c>
       <c r="L83" s="3" t="s">
@@ -6292,13 +6549,16 @@
         <v>179</v>
       </c>
       <c r="P83" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q83" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U83" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="84" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>391</v>
       </c>
@@ -6309,7 +6569,7 @@
         <v>469</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>14</v>
@@ -6323,7 +6583,7 @@
       <c r="H84" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="J84" s="10" t="s">
+      <c r="J84" s="9" t="s">
         <v>561</v>
       </c>
       <c r="L84" s="3" t="s">
@@ -6339,13 +6599,16 @@
         <v>180</v>
       </c>
       <c r="P84" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q84" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U84" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="85" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>410</v>
       </c>
@@ -6356,7 +6619,7 @@
         <v>483</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>14</v>
@@ -6386,13 +6649,16 @@
         <v>197</v>
       </c>
       <c r="P85" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q85" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U85" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="86" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>412</v>
       </c>
@@ -6403,7 +6669,7 @@
         <v>484</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>14</v>
@@ -6433,13 +6699,16 @@
         <v>198</v>
       </c>
       <c r="P86" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q86" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U86" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="87" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
         <v>116</v>
       </c>
@@ -6447,7 +6716,7 @@
         <v>327</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>133</v>
@@ -6461,7 +6730,7 @@
       <c r="H87" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="J87" s="10" t="s">
+      <c r="J87" s="9" t="s">
         <v>588</v>
       </c>
       <c r="L87" s="3" t="s">
@@ -6476,8 +6745,11 @@
       <c r="O87" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U87" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="88" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>413</v>
       </c>
@@ -6488,7 +6760,7 @@
         <v>485</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>133</v>
@@ -6515,16 +6787,19 @@
         <v>20</v>
       </c>
       <c r="O88" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="P88" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q88" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U88" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>28</v>
       </c>
@@ -6535,7 +6810,7 @@
         <v>25</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>600</v>
+        <v>630</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>23</v>
@@ -6560,13 +6835,17 @@
         <v>20</v>
       </c>
       <c r="P89" s="3" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="Q89" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+      <c r="U89" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="W89" s="8"/>
+    </row>
+    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>32</v>
       </c>
@@ -6577,7 +6856,7 @@
         <v>25</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>600</v>
+        <v>629</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>23</v>
@@ -6602,13 +6881,16 @@
         <v>20</v>
       </c>
       <c r="P90" s="3" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="Q90" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+      <c r="U90" s="3" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="91" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
         <v>33</v>
       </c>
@@ -6616,7 +6898,7 @@
         <v>436</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>601</v>
+        <v>631</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>34</v>
@@ -6644,13 +6926,16 @@
         <v>37</v>
       </c>
       <c r="P91" s="3" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="Q91" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+      <c r="U91" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="92" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>337</v>
       </c>
@@ -6661,7 +6946,7 @@
         <v>435</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>14</v>
@@ -6689,13 +6974,16 @@
         <v>140</v>
       </c>
       <c r="P92" s="3" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="Q92" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+      <c r="U92" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="93" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
         <v>118</v>
       </c>
@@ -6703,7 +6991,7 @@
         <v>486</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>602</v>
+        <v>632</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>34</v>
@@ -6730,8 +7018,11 @@
       <c r="O93" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U93" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
         <v>132</v>
       </c>
@@ -6739,7 +7030,7 @@
         <v>495</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>603</v>
+        <v>633</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>34</v>
@@ -6754,7 +7045,7 @@
         <v>305</v>
       </c>
       <c r="J94" s="3"/>
-      <c r="L94" s="9" t="s">
+      <c r="L94" s="3" t="s">
         <v>497</v>
       </c>
       <c r="M94" s="3" t="s">
@@ -6764,8 +7055,11 @@
         <v>20</v>
       </c>
       <c r="O94"/>
-    </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U94" s="3" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="95" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
         <v>56</v>
       </c>
@@ -6773,7 +7067,7 @@
         <v>442</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>133</v>
@@ -6800,16 +7094,19 @@
         <v>20</v>
       </c>
       <c r="O95" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="P95" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q95" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U95" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="96" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>382</v>
       </c>
@@ -6820,7 +7117,7 @@
         <v>461</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>133</v>
@@ -6847,16 +7144,19 @@
         <v>20</v>
       </c>
       <c r="O96" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="P96" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q96" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U96" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="97" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>400</v>
       </c>
@@ -6867,7 +7167,7 @@
         <v>478</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>14</v>
@@ -6881,7 +7181,7 @@
       <c r="H97" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="J97" s="10" t="s">
+      <c r="J97" s="9" t="s">
         <v>570</v>
       </c>
       <c r="L97" s="3" t="s">
@@ -6897,13 +7197,16 @@
         <v>189</v>
       </c>
       <c r="P97" s="3" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="Q97" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+      <c r="U97" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="98" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>401</v>
       </c>
@@ -6914,7 +7217,7 @@
         <v>478</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>14</v>
@@ -6928,7 +7231,7 @@
       <c r="H98" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="J98" s="10" t="s">
+      <c r="J98" s="9" t="s">
         <v>571</v>
       </c>
       <c r="L98" s="3" t="s">
@@ -6944,13 +7247,16 @@
         <v>190</v>
       </c>
       <c r="P98" s="3" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="Q98" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+      <c r="U98" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="99" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>402</v>
       </c>
@@ -6961,7 +7267,7 @@
         <v>479</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>133</v>
@@ -6975,7 +7281,7 @@
       <c r="H99" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="J99" s="10" t="s">
+      <c r="J99" s="9" t="s">
         <v>572</v>
       </c>
       <c r="L99" s="3" t="s">
@@ -6991,13 +7297,16 @@
         <v>191</v>
       </c>
       <c r="P99" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q99" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U99" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="100" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>409</v>
       </c>
@@ -7008,7 +7317,7 @@
         <v>211</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>133</v>
@@ -7038,13 +7347,16 @@
         <v>196</v>
       </c>
       <c r="P100" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q100" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U100" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="101" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>418</v>
       </c>
@@ -7055,7 +7367,7 @@
         <v>489</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>14</v>
@@ -7085,13 +7397,16 @@
         <v>203</v>
       </c>
       <c r="P101" s="3" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="Q101" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+      <c r="U101" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="102" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B102" s="3" t="s">
         <v>122</v>
       </c>
@@ -7099,7 +7414,7 @@
         <v>490</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>600</v>
+        <v>630</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>133</v>
@@ -7126,17 +7441,23 @@
         <v>20</v>
       </c>
       <c r="O102" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="P102" s="3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="Q102" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="U102" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="103" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D103" s="8"/>
+    </row>
+    <row r="104" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X104" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>

</xml_diff>

<commit_message>
cambios en el dashboard
</commit_message>
<xml_diff>
--- a/src/assets/EQUIPOS.xlsx
+++ b/src/assets/EQUIPOS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A79754-4E62-46C8-81C6-C1E3D63D7E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1376AB55-3200-4EB2-A527-A72947F9D0E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1523,21 +1523,12 @@
     <t>ARRIVA\jefalmcun</t>
   </si>
   <si>
-    <t>CROWNCUN\asistllaves</t>
-  </si>
-  <si>
     <t>CROWNCUN\amadellaves2</t>
   </si>
   <si>
-    <t>CROWNCUN\ama de llaves</t>
-  </si>
-  <si>
     <t>LOCAL\apublicas</t>
   </si>
   <si>
-    <t>CROWNCUN\chefejecutivo</t>
-  </si>
-  <si>
     <t>Room Service</t>
   </si>
   <si>
@@ -1926,6 +1917,15 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>ARRIVA\asisllavescun</t>
+  </si>
+  <si>
+    <t>ARRIVA\chefejecutivocun</t>
+  </si>
+  <si>
+    <t>ARRIVA\jefeamallavescun</t>
   </si>
 </sst>
 </file>
@@ -2165,15 +2165,9 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EF8ACE9A-3DC4-4577-9E29-4CEAA3B671E9}" name="Tabla1" displayName="Tabla1" ref="A1:U102" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
-  <autoFilter ref="A1:U102" xr:uid="{EF8ACE9A-3DC4-4577-9E29-4CEAA3B671E9}">
-    <filterColumn colId="20">
-      <filters>
-        <filter val="X"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T102">
-    <sortCondition ref="M1:M102"/>
+  <autoFilter ref="A1:U102" xr:uid="{EF8ACE9A-3DC4-4577-9E29-4CEAA3B671E9}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:U94">
+    <sortCondition ref="U1:U102"/>
   </sortState>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{59771C38-00B0-4DC3-A168-A8045865F88D}" name="Etiqueta" dataDxfId="20"/>
@@ -2526,8 +2520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="W89" sqref="W89"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2602,25 +2596,25 @@
         <v>11</v>
       </c>
       <c r="P1" s="7" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>617</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="T1" s="2" t="s">
         <v>618</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>619</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>620</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>621</v>
-      </c>
       <c r="U1" s="7" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>338</v>
       </c>
@@ -2631,7 +2625,7 @@
         <v>437</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>14</v>
@@ -2646,7 +2640,7 @@
         <v>219</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>506</v>
+        <v>635</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>311</v>
@@ -2661,16 +2655,16 @@
         <v>141</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>344</v>
       </c>
@@ -2678,10 +2672,10 @@
         <v>46</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>14</v>
@@ -2696,7 +2690,7 @@
         <v>220</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>311</v>
@@ -2711,24 +2705,24 @@
         <v>142</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>14</v>
@@ -2743,7 +2737,7 @@
         <v>221</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>311</v>
@@ -2758,16 +2752,16 @@
         <v>143</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>345</v>
       </c>
@@ -2778,7 +2772,7 @@
         <v>438</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>133</v>
@@ -2793,7 +2787,7 @@
         <v>222</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>311</v>
@@ -2808,16 +2802,16 @@
         <v>144</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>347</v>
       </c>
@@ -2825,10 +2819,10 @@
         <v>49</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>14</v>
@@ -2843,7 +2837,7 @@
         <v>223</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>311</v>
@@ -2858,16 +2852,16 @@
         <v>145</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>50</v>
       </c>
@@ -2875,7 +2869,7 @@
         <v>439</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>14</v>
@@ -2890,7 +2884,7 @@
         <v>224</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>311</v>
@@ -2905,13 +2899,13 @@
         <v>146</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -2925,7 +2919,7 @@
         <v>440</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>14</v>
@@ -2940,7 +2934,7 @@
         <v>225</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>312</v>
@@ -2953,10 +2947,10 @@
       </c>
       <c r="O8"/>
       <c r="U8" s="3" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>349</v>
       </c>
@@ -2964,10 +2958,10 @@
         <v>52</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>14</v>
@@ -2982,7 +2976,7 @@
         <v>226</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>312</v>
@@ -2997,16 +2991,16 @@
         <v>147</v>
       </c>
       <c r="P9" s="10" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>350</v>
       </c>
@@ -3014,10 +3008,10 @@
         <v>53</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>133</v>
@@ -3032,7 +3026,7 @@
         <v>227</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>312</v>
@@ -3047,16 +3041,16 @@
         <v>148</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>352</v>
       </c>
@@ -3064,10 +3058,10 @@
         <v>54</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>14</v>
@@ -3082,7 +3076,7 @@
         <v>228</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>312</v>
@@ -3097,16 +3091,16 @@
         <v>149</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U11" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>55</v>
       </c>
@@ -3114,7 +3108,7 @@
         <v>441</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>133</v>
@@ -3129,7 +3123,7 @@
         <v>229</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>312</v>
@@ -3144,16 +3138,16 @@
         <v>150</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U12" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>356</v>
       </c>
@@ -3164,7 +3158,7 @@
         <v>445</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>14</v>
@@ -3179,7 +3173,7 @@
         <v>232</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>315</v>
@@ -3194,10 +3188,10 @@
         <v>152</v>
       </c>
       <c r="U13" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>357</v>
       </c>
@@ -3208,7 +3202,7 @@
         <v>446</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>14</v>
@@ -3223,7 +3217,7 @@
         <v>233</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>315</v>
@@ -3238,16 +3232,16 @@
         <v>153</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U14" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>358</v>
       </c>
@@ -3258,7 +3252,7 @@
         <v>447</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>133</v>
@@ -3273,7 +3267,7 @@
         <v>234</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>315</v>
@@ -3288,16 +3282,16 @@
         <v>154</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U15" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>359</v>
       </c>
@@ -3305,10 +3299,10 @@
         <v>61</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>133</v>
@@ -3323,7 +3317,7 @@
         <v>235</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>315</v>
@@ -3336,16 +3330,16 @@
       </c>
       <c r="O16"/>
       <c r="P16" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U16" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>360</v>
       </c>
@@ -3356,7 +3350,7 @@
         <v>448</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>133</v>
@@ -3371,7 +3365,7 @@
         <v>236</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>315</v>
@@ -3383,19 +3377,19 @@
         <v>20</v>
       </c>
       <c r="O17" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U17" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>362</v>
       </c>
@@ -3406,7 +3400,7 @@
         <v>449</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>14</v>
@@ -3421,7 +3415,7 @@
         <v>237</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>315</v>
@@ -3436,16 +3430,16 @@
         <v>155</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U18" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
@@ -3456,7 +3450,7 @@
         <v>428</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>14</v>
@@ -3486,16 +3480,16 @@
         <v>21</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U19" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>330</v>
       </c>
@@ -3506,7 +3500,7 @@
         <v>429</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>14</v>
@@ -3536,16 +3530,16 @@
         <v>134</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U20" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>332</v>
       </c>
@@ -3556,7 +3550,7 @@
         <v>430</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>14</v>
@@ -3586,16 +3580,16 @@
         <v>135</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q21" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U21" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>354</v>
       </c>
@@ -3606,7 +3600,7 @@
         <v>443</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>133</v>
@@ -3621,7 +3615,7 @@
         <v>231</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>314</v>
@@ -3636,16 +3630,16 @@
         <v>151</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U22" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>369</v>
       </c>
@@ -3656,7 +3650,7 @@
         <v>454</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>14</v>
@@ -3671,7 +3665,7 @@
         <v>243</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="L23" s="3" t="s">
         <v>317</v>
@@ -3686,16 +3680,16 @@
         <v>161</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U23" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>370</v>
       </c>
@@ -3706,7 +3700,7 @@
         <v>454</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>14</v>
@@ -3721,7 +3715,7 @@
         <v>244</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>317</v>
@@ -3736,16 +3730,16 @@
         <v>162</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U24" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>371</v>
       </c>
@@ -3756,7 +3750,7 @@
         <v>444</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>14</v>
@@ -3771,7 +3765,7 @@
         <v>245</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="L25" s="3" t="s">
         <v>317</v>
@@ -3786,24 +3780,24 @@
         <v>163</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U25" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>72</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>133</v>
@@ -3818,7 +3812,7 @@
         <v>246</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>318</v>
@@ -3831,16 +3825,16 @@
       </c>
       <c r="O26"/>
       <c r="P26" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q26" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U26" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>373</v>
       </c>
@@ -3848,10 +3842,10 @@
         <v>73</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>14</v>
@@ -3866,7 +3860,7 @@
         <v>247</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="L27" s="3" t="s">
         <v>318</v>
@@ -3881,16 +3875,16 @@
         <v>164</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q27" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U27" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>74</v>
       </c>
@@ -3898,7 +3892,7 @@
         <v>455</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>14</v>
@@ -3913,7 +3907,7 @@
         <v>248</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="L28" s="3" t="s">
         <v>318</v>
@@ -3928,16 +3922,16 @@
         <v>165</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q28" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U28" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>374</v>
       </c>
@@ -3946,7 +3940,7 @@
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>14</v>
@@ -3972,10 +3966,10 @@
       </c>
       <c r="O29"/>
       <c r="U29" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>375</v>
       </c>
@@ -3986,7 +3980,7 @@
         <v>456</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>133</v>
@@ -4001,7 +3995,7 @@
         <v>250</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="L30" s="3" t="s">
         <v>210</v>
@@ -4013,19 +4007,19 @@
         <v>20</v>
       </c>
       <c r="O30" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q30" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U30" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>376</v>
       </c>
@@ -4036,7 +4030,7 @@
         <v>457</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>133</v>
@@ -4051,7 +4045,7 @@
         <v>251</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="L31" s="3" t="s">
         <v>319</v>
@@ -4066,16 +4060,16 @@
         <v>166</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U31" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>377</v>
       </c>
@@ -4083,10 +4077,10 @@
         <v>78</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>14</v>
@@ -4101,7 +4095,7 @@
         <v>252</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="L32" s="3" t="s">
         <v>318</v>
@@ -4116,16 +4110,16 @@
         <v>167</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q32" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U32" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>378</v>
       </c>
@@ -4134,7 +4128,7 @@
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>14</v>
@@ -4149,7 +4143,7 @@
         <v>253</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="L33" s="3" t="s">
         <v>318</v>
@@ -4164,16 +4158,16 @@
         <v>168</v>
       </c>
       <c r="P33" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q33" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U33" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>379</v>
       </c>
@@ -4184,7 +4178,7 @@
         <v>458</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>14</v>
@@ -4199,7 +4193,7 @@
         <v>254</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="L34" s="3" t="s">
         <v>318</v>
@@ -4214,16 +4208,16 @@
         <v>169</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q34" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U34" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>383</v>
       </c>
@@ -4234,7 +4228,7 @@
         <v>462</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>14</v>
@@ -4249,7 +4243,7 @@
         <v>259</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="L35" s="3" t="s">
         <v>318</v>
@@ -4264,16 +4258,16 @@
         <v>173</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q35" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U35" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>384</v>
       </c>
@@ -4284,7 +4278,7 @@
         <v>463</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>14</v>
@@ -4299,7 +4293,7 @@
         <v>260</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="L36" s="3" t="s">
         <v>318</v>
@@ -4314,16 +4308,16 @@
         <v>174</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q36" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U36" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>392</v>
       </c>
@@ -4334,7 +4328,7 @@
         <v>470</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>14</v>
@@ -4349,7 +4343,7 @@
         <v>267</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="L37" s="3" t="s">
         <v>318</v>
@@ -4364,16 +4358,16 @@
         <v>181</v>
       </c>
       <c r="P37" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q37" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U37" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>110</v>
       </c>
@@ -4381,7 +4375,7 @@
         <v>481</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>14</v>
@@ -4396,7 +4390,7 @@
         <v>283</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>26</v>
@@ -4411,16 +4405,16 @@
         <v>195</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q38" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U38" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
         <v>111</v>
       </c>
@@ -4428,7 +4422,7 @@
         <v>481</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>133</v>
@@ -4443,7 +4437,7 @@
         <v>284</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>26</v>
@@ -4456,16 +4450,16 @@
       </c>
       <c r="O39"/>
       <c r="P39" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q39" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U39" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>408</v>
       </c>
@@ -4476,7 +4470,7 @@
         <v>482</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>133</v>
@@ -4491,7 +4485,7 @@
         <v>285</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="L40" s="3" t="s">
         <v>26</v>
@@ -4503,19 +4497,19 @@
         <v>20</v>
       </c>
       <c r="O40" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="P40" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q40" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U40" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>342</v>
       </c>
@@ -4526,7 +4520,7 @@
         <v>496</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>133</v>
@@ -4541,7 +4535,7 @@
         <v>340</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="L41" s="3" t="s">
         <v>318</v>
@@ -4556,22 +4550,22 @@
         <v>341</v>
       </c>
       <c r="P41" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q41" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U41" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
         <v>421</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>133</v>
@@ -4599,16 +4593,16 @@
         <v>422</v>
       </c>
       <c r="P42" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q42" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U42" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>333</v>
       </c>
@@ -4619,7 +4613,7 @@
         <v>431</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>14</v>
@@ -4634,7 +4628,7 @@
         <v>214</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>502</v>
+        <v>634</v>
       </c>
       <c r="L43" s="3" t="s">
         <v>310</v>
@@ -4649,16 +4643,16 @@
         <v>136</v>
       </c>
       <c r="P43" s="3" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="Q43" s="3" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="U43" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>41</v>
       </c>
@@ -4666,7 +4660,7 @@
         <v>432</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>14</v>
@@ -4681,7 +4675,7 @@
         <v>215</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="L44" s="3" t="s">
         <v>310</v>
@@ -4696,16 +4690,16 @@
         <v>137</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q44" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U44" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>334</v>
       </c>
@@ -4716,7 +4710,7 @@
         <v>433</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>14</v>
@@ -4731,7 +4725,7 @@
         <v>216</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>504</v>
+        <v>636</v>
       </c>
       <c r="L45" s="3" t="s">
         <v>310</v>
@@ -4746,16 +4740,16 @@
         <v>138</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q45" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U45" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>335</v>
       </c>
@@ -4766,7 +4760,7 @@
         <v>434</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>14</v>
@@ -4781,7 +4775,7 @@
         <v>217</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="L46" s="3" t="s">
         <v>310</v>
@@ -4796,16 +4790,16 @@
         <v>139</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q46" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U46" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>363</v>
       </c>
@@ -4816,7 +4810,7 @@
         <v>450</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>14</v>
@@ -4831,7 +4825,7 @@
         <v>238</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="L47" s="3" t="s">
         <v>316</v>
@@ -4846,16 +4840,16 @@
         <v>156</v>
       </c>
       <c r="P47" s="3" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="Q47" s="3" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="U47" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>364</v>
       </c>
@@ -4866,7 +4860,7 @@
         <v>451</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>14</v>
@@ -4881,7 +4875,7 @@
         <v>239</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="L48" s="3" t="s">
         <v>316</v>
@@ -4896,24 +4890,24 @@
         <v>157</v>
       </c>
       <c r="P48" s="3" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="Q48" s="3" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="U48" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>14</v>
@@ -4928,7 +4922,7 @@
         <v>240</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="L49" s="3" t="s">
         <v>316</v>
@@ -4943,16 +4937,16 @@
         <v>158</v>
       </c>
       <c r="P49" s="3" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="Q49" s="3" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="U49" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>366</v>
       </c>
@@ -4963,7 +4957,7 @@
         <v>452</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>14</v>
@@ -4978,7 +4972,7 @@
         <v>241</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="L50" s="3" t="s">
         <v>316</v>
@@ -4993,16 +4987,16 @@
         <v>159</v>
       </c>
       <c r="P50" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q50" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U50" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>368</v>
       </c>
@@ -5013,7 +5007,7 @@
         <v>453</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>14</v>
@@ -5028,7 +5022,7 @@
         <v>242</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="L51" s="3" t="s">
         <v>316</v>
@@ -5043,16 +5037,16 @@
         <v>160</v>
       </c>
       <c r="P51" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q51" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U51" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>380</v>
       </c>
@@ -5063,7 +5057,7 @@
         <v>459</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>133</v>
@@ -5078,7 +5072,7 @@
         <v>255</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="L52" s="3" t="s">
         <v>320</v>
@@ -5093,16 +5087,16 @@
         <v>170</v>
       </c>
       <c r="P52" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q52" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U52" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>385</v>
       </c>
@@ -5113,7 +5107,7 @@
         <v>464</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>14</v>
@@ -5128,7 +5122,7 @@
         <v>261</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="L53" s="3" t="s">
         <v>323</v>
@@ -5143,16 +5137,16 @@
         <v>175</v>
       </c>
       <c r="P53" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q53" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U53" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>393</v>
       </c>
@@ -5163,7 +5157,7 @@
         <v>476</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>14</v>
@@ -5178,7 +5172,7 @@
         <v>268</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="L54" s="3" t="s">
         <v>325</v>
@@ -5193,16 +5187,16 @@
         <v>182</v>
       </c>
       <c r="P54" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q54" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U54" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>394</v>
       </c>
@@ -5213,7 +5207,7 @@
         <v>474</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>14</v>
@@ -5228,7 +5222,7 @@
         <v>269</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="L55" s="3" t="s">
         <v>325</v>
@@ -5243,16 +5237,16 @@
         <v>183</v>
       </c>
       <c r="P55" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q55" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U55" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>395</v>
       </c>
@@ -5263,7 +5257,7 @@
         <v>475</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>14</v>
@@ -5278,7 +5272,7 @@
         <v>270</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="L56" s="3" t="s">
         <v>325</v>
@@ -5293,16 +5287,16 @@
         <v>184</v>
       </c>
       <c r="P56" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q56" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U56" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>396</v>
       </c>
@@ -5313,7 +5307,7 @@
         <v>473</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>14</v>
@@ -5328,7 +5322,7 @@
         <v>271</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="L57" s="3" t="s">
         <v>325</v>
@@ -5343,16 +5337,16 @@
         <v>185</v>
       </c>
       <c r="P57" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q57" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U57" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>397</v>
       </c>
@@ -5363,7 +5357,7 @@
         <v>472</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>14</v>
@@ -5378,7 +5372,7 @@
         <v>272</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="L58" s="3" t="s">
         <v>325</v>
@@ -5393,16 +5387,16 @@
         <v>186</v>
       </c>
       <c r="P58" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q58" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U58" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="59" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>398</v>
       </c>
@@ -5413,7 +5407,7 @@
         <v>471</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>14</v>
@@ -5428,7 +5422,7 @@
         <v>273</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="L59" s="3" t="s">
         <v>325</v>
@@ -5443,16 +5437,16 @@
         <v>187</v>
       </c>
       <c r="P59" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q59" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U59" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="60" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>399</v>
       </c>
@@ -5463,7 +5457,7 @@
         <v>477</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>14</v>
@@ -5478,7 +5472,7 @@
         <v>274</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="L60" s="3" t="s">
         <v>325</v>
@@ -5493,24 +5487,24 @@
         <v>188</v>
       </c>
       <c r="P60" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q60" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U60" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="61" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>14</v>
@@ -5538,16 +5532,16 @@
         <v>192</v>
       </c>
       <c r="P61" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q61" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U61" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="62" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>405</v>
       </c>
@@ -5555,10 +5549,10 @@
         <v>105</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>133</v>
@@ -5573,7 +5567,7 @@
         <v>279</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="L62" s="3" t="s">
         <v>327</v>
@@ -5586,18 +5580,18 @@
       </c>
       <c r="O62"/>
       <c r="U62" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="63" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
         <v>106</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>133</v>
@@ -5612,7 +5606,7 @@
         <v>280</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="L63" s="3" t="s">
         <v>327</v>
@@ -5625,7 +5619,7 @@
       </c>
       <c r="O63"/>
       <c r="U63" s="3" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.25">
@@ -5633,10 +5627,10 @@
         <v>107</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>14</v>
@@ -5646,7 +5640,7 @@
       </c>
       <c r="H64" s="1"/>
       <c r="J64" s="3" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="L64" s="3" t="s">
         <v>327</v>
@@ -5661,18 +5655,18 @@
         <v>193</v>
       </c>
       <c r="U64" s="3" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="65" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
         <v>108</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>14</v>
@@ -5687,7 +5681,7 @@
         <v>281</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="L65" s="3" t="s">
         <v>327</v>
@@ -5702,10 +5696,10 @@
         <v>194</v>
       </c>
       <c r="U65" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="66" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
         <v>109</v>
       </c>
@@ -5713,7 +5707,7 @@
         <v>480</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>14</v>
@@ -5728,7 +5722,7 @@
         <v>282</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="L66" s="3" t="s">
         <v>327</v>
@@ -5740,19 +5734,19 @@
         <v>20</v>
       </c>
       <c r="O66" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="P66" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q66" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U66" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="67" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>414</v>
       </c>
@@ -5763,7 +5757,7 @@
         <v>487</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>14</v>
@@ -5778,7 +5772,7 @@
         <v>292</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="L67" s="3" t="s">
         <v>316</v>
@@ -5793,16 +5787,16 @@
         <v>201</v>
       </c>
       <c r="P67" s="3" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="Q67" s="3" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="U67" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="68" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>417</v>
       </c>
@@ -5813,7 +5807,7 @@
         <v>488</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>14</v>
@@ -5828,7 +5822,7 @@
         <v>293</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="L68" s="3" t="s">
         <v>329</v>
@@ -5843,16 +5837,16 @@
         <v>202</v>
       </c>
       <c r="P68" s="3" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="Q68" s="3" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="U68" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="69" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>381</v>
       </c>
@@ -5863,7 +5857,7 @@
         <v>460</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>133</v>
@@ -5878,7 +5872,7 @@
         <v>256</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="L69" s="3" t="s">
         <v>321</v>
@@ -5893,22 +5887,22 @@
         <v>171</v>
       </c>
       <c r="P69" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q69" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U69" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="70" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
         <v>84</v>
       </c>
       <c r="C70" s="4"/>
       <c r="D70" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>133</v>
@@ -5923,7 +5917,7 @@
         <v>258</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="L70" s="3" t="s">
         <v>322</v>
@@ -5938,22 +5932,22 @@
         <v>172</v>
       </c>
       <c r="P70" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q70" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U70" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="71" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C71" s="4"/>
       <c r="D71" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>133</v>
@@ -5968,7 +5962,7 @@
         <v>296</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="L71" s="3" t="s">
         <v>322</v>
@@ -5980,27 +5974,27 @@
         <v>20</v>
       </c>
       <c r="O71" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="P71" s="11" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="Q71" s="3" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="U71" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="72" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
         <v>124</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>14</v>
@@ -6015,7 +6009,7 @@
         <v>297</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="L72" s="3" t="s">
         <v>322</v>
@@ -6030,16 +6024,16 @@
         <v>204</v>
       </c>
       <c r="P72" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q72" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U72" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="73" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
         <v>125</v>
       </c>
@@ -6047,7 +6041,7 @@
         <v>491</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>133</v>
@@ -6062,7 +6056,7 @@
         <v>298</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="L73" s="3" t="s">
         <v>322</v>
@@ -6077,16 +6071,16 @@
         <v>205</v>
       </c>
       <c r="P73" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q73" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U73" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="74" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
         <v>126</v>
       </c>
@@ -6094,7 +6088,7 @@
         <v>492</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>133</v>
@@ -6109,7 +6103,7 @@
         <v>299</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="L74" s="3" t="s">
         <v>322</v>
@@ -6124,16 +6118,16 @@
         <v>206</v>
       </c>
       <c r="P74" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q74" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U74" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="75" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
         <v>127</v>
       </c>
@@ -6141,7 +6135,7 @@
         <v>493</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>14</v>
@@ -6156,7 +6150,7 @@
         <v>300</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="L75" s="3" t="s">
         <v>322</v>
@@ -6169,24 +6163,24 @@
       </c>
       <c r="O75"/>
       <c r="P75" s="3" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="Q75" s="3" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="U75" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="76" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
         <v>128</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>14</v>
@@ -6201,7 +6195,7 @@
         <v>301</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="L76" s="3" t="s">
         <v>322</v>
@@ -6216,24 +6210,24 @@
         <v>207</v>
       </c>
       <c r="P76" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q76" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U76" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="77" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="s">
         <v>129</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>14</v>
@@ -6248,7 +6242,7 @@
         <v>302</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="L77" s="3" t="s">
         <v>322</v>
@@ -6261,18 +6255,18 @@
       </c>
       <c r="O77"/>
       <c r="U77" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
         <v>130</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>133</v>
@@ -6287,7 +6281,7 @@
         <v>303</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="L78" s="3" t="s">
         <v>322</v>
@@ -6302,16 +6296,16 @@
         <v>208</v>
       </c>
       <c r="P78" s="3" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="Q78" s="3" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="U78" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="79" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
         <v>131</v>
       </c>
@@ -6319,7 +6313,7 @@
         <v>494</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>14</v>
@@ -6334,7 +6328,7 @@
         <v>304</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="L79" s="3" t="s">
         <v>322</v>
@@ -6349,16 +6343,16 @@
         <v>209</v>
       </c>
       <c r="P79" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q79" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U79" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>387</v>
       </c>
@@ -6369,7 +6363,7 @@
         <v>465</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>14</v>
@@ -6384,7 +6378,7 @@
         <v>262</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="L80" s="3" t="s">
         <v>324</v>
@@ -6399,16 +6393,16 @@
         <v>176</v>
       </c>
       <c r="P80" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q80" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U80" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="81" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>388</v>
       </c>
@@ -6419,7 +6413,7 @@
         <v>466</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>14</v>
@@ -6434,7 +6428,7 @@
         <v>263</v>
       </c>
       <c r="J81" s="9" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="L81" s="3" t="s">
         <v>324</v>
@@ -6449,16 +6443,16 @@
         <v>177</v>
       </c>
       <c r="P81" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q81" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U81" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="82" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>389</v>
       </c>
@@ -6469,7 +6463,7 @@
         <v>467</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>14</v>
@@ -6484,7 +6478,7 @@
         <v>264</v>
       </c>
       <c r="J82" s="9" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="L82" s="3" t="s">
         <v>324</v>
@@ -6499,16 +6493,16 @@
         <v>178</v>
       </c>
       <c r="P82" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q82" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U82" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="83" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>390</v>
       </c>
@@ -6519,7 +6513,7 @@
         <v>468</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>133</v>
@@ -6534,7 +6528,7 @@
         <v>265</v>
       </c>
       <c r="J83" s="9" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="L83" s="3" t="s">
         <v>324</v>
@@ -6549,16 +6543,16 @@
         <v>179</v>
       </c>
       <c r="P83" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q83" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U83" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="84" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>391</v>
       </c>
@@ -6569,7 +6563,7 @@
         <v>469</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>14</v>
@@ -6584,7 +6578,7 @@
         <v>266</v>
       </c>
       <c r="J84" s="9" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="L84" s="3" t="s">
         <v>324</v>
@@ -6599,16 +6593,16 @@
         <v>180</v>
       </c>
       <c r="P84" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q84" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U84" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="85" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>410</v>
       </c>
@@ -6619,7 +6613,7 @@
         <v>483</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>14</v>
@@ -6634,7 +6628,7 @@
         <v>287</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="L85" s="3" t="s">
         <v>328</v>
@@ -6649,16 +6643,16 @@
         <v>197</v>
       </c>
       <c r="P85" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q85" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U85" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="86" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>412</v>
       </c>
@@ -6669,7 +6663,7 @@
         <v>484</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>14</v>
@@ -6684,7 +6678,7 @@
         <v>288</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="L86" s="3" t="s">
         <v>328</v>
@@ -6699,16 +6693,16 @@
         <v>198</v>
       </c>
       <c r="P86" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q86" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U86" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="87" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
         <v>116</v>
       </c>
@@ -6716,7 +6710,7 @@
         <v>327</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>133</v>
@@ -6731,7 +6725,7 @@
         <v>289</v>
       </c>
       <c r="J87" s="9" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="L87" s="3" t="s">
         <v>327</v>
@@ -6746,10 +6740,10 @@
         <v>199</v>
       </c>
       <c r="U87" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="88" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>413</v>
       </c>
@@ -6760,7 +6754,7 @@
         <v>485</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>133</v>
@@ -6775,7 +6769,7 @@
         <v>290</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="L88" s="3" t="s">
         <v>328</v>
@@ -6787,16 +6781,16 @@
         <v>20</v>
       </c>
       <c r="O88" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="P88" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q88" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U88" s="3" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="89" spans="1:23" x14ac:dyDescent="0.25">
@@ -6810,7 +6804,7 @@
         <v>25</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>23</v>
@@ -6835,13 +6829,13 @@
         <v>20</v>
       </c>
       <c r="P89" s="3" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="Q89" s="3" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="U89" s="3" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="W89" s="8"/>
     </row>
@@ -6856,7 +6850,7 @@
         <v>25</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>23</v>
@@ -6881,16 +6875,16 @@
         <v>20</v>
       </c>
       <c r="P90" s="3" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="Q90" s="3" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="U90" s="3" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="91" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
         <v>33</v>
       </c>
@@ -6898,7 +6892,7 @@
         <v>436</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>34</v>
@@ -6926,16 +6920,16 @@
         <v>37</v>
       </c>
       <c r="P91" s="3" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="Q91" s="3" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="U91" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="92" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>337</v>
       </c>
@@ -6946,7 +6940,7 @@
         <v>435</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>14</v>
@@ -6974,16 +6968,16 @@
         <v>140</v>
       </c>
       <c r="P92" s="3" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="Q92" s="3" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="U92" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="93" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
         <v>118</v>
       </c>
@@ -6991,7 +6985,7 @@
         <v>486</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>34</v>
@@ -7019,7 +7013,7 @@
         <v>200</v>
       </c>
       <c r="U93" s="3" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="94" spans="1:23" x14ac:dyDescent="0.25">
@@ -7030,7 +7024,7 @@
         <v>495</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>34</v>
@@ -7056,10 +7050,10 @@
       </c>
       <c r="O94"/>
       <c r="U94" s="3" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="95" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
         <v>56</v>
       </c>
@@ -7067,7 +7061,7 @@
         <v>442</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>133</v>
@@ -7082,7 +7076,7 @@
         <v>230</v>
       </c>
       <c r="J95" s="3" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="L95" s="3" t="s">
         <v>313</v>
@@ -7094,19 +7088,19 @@
         <v>20</v>
       </c>
       <c r="O95" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="P95" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q95" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U95" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="96" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>382</v>
       </c>
@@ -7117,7 +7111,7 @@
         <v>461</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>133</v>
@@ -7132,7 +7126,7 @@
         <v>257</v>
       </c>
       <c r="J96" s="3" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="L96" s="3" t="s">
         <v>313</v>
@@ -7144,19 +7138,19 @@
         <v>20</v>
       </c>
       <c r="O96" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="P96" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q96" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U96" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="97" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="97" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>400</v>
       </c>
@@ -7167,7 +7161,7 @@
         <v>478</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>14</v>
@@ -7182,7 +7176,7 @@
         <v>275</v>
       </c>
       <c r="J97" s="9" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="L97" s="3" t="s">
         <v>326</v>
@@ -7197,16 +7191,16 @@
         <v>189</v>
       </c>
       <c r="P97" s="3" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="Q97" s="3" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="U97" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="98" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>401</v>
       </c>
@@ -7217,7 +7211,7 @@
         <v>478</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>14</v>
@@ -7232,7 +7226,7 @@
         <v>276</v>
       </c>
       <c r="J98" s="9" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="L98" s="3" t="s">
         <v>326</v>
@@ -7247,16 +7241,16 @@
         <v>190</v>
       </c>
       <c r="P98" s="3" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="Q98" s="3" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="U98" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="99" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="99" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>402</v>
       </c>
@@ -7267,7 +7261,7 @@
         <v>479</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>133</v>
@@ -7282,7 +7276,7 @@
         <v>277</v>
       </c>
       <c r="J99" s="9" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="L99" s="3" t="s">
         <v>326</v>
@@ -7297,16 +7291,16 @@
         <v>191</v>
       </c>
       <c r="P99" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q99" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U99" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="100" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="100" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>409</v>
       </c>
@@ -7317,7 +7311,7 @@
         <v>211</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>133</v>
@@ -7332,7 +7326,7 @@
         <v>286</v>
       </c>
       <c r="J100" s="3" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="L100" s="3" t="s">
         <v>211</v>
@@ -7347,16 +7341,16 @@
         <v>196</v>
       </c>
       <c r="P100" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q100" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U100" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="101" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="101" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>418</v>
       </c>
@@ -7367,7 +7361,7 @@
         <v>489</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>14</v>
@@ -7382,7 +7376,7 @@
         <v>294</v>
       </c>
       <c r="J101" s="3" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="L101" s="3" t="s">
         <v>313</v>
@@ -7397,16 +7391,16 @@
         <v>203</v>
       </c>
       <c r="P101" s="3" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="Q101" s="3" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="U101" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="102" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="102" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B102" s="3" t="s">
         <v>122</v>
       </c>
@@ -7414,7 +7408,7 @@
         <v>490</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>133</v>
@@ -7429,7 +7423,7 @@
         <v>295</v>
       </c>
       <c r="J102" s="3" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="L102" s="3" t="s">
         <v>313</v>
@@ -7441,16 +7435,16 @@
         <v>20</v>
       </c>
       <c r="O102" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="P102" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q102" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="U102" s="3" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="103" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
cambio en los archivos
</commit_message>
<xml_diff>
--- a/src/assets/EQUIPOS.xlsx
+++ b/src/assets/EQUIPOS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6ACA6F5-50B8-435C-9601-0387B5F5DF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98970F63-6F33-47B2-B909-65DFE29E5917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="670">
   <si>
     <t>Etiqueta</t>
   </si>
@@ -1521,9 +1521,6 @@
   </si>
   <si>
     <t>CROWNCUN\amadellaves2</t>
-  </si>
-  <si>
-    <t>LOCAL\apublicas</t>
   </si>
   <si>
     <t>Room Service</t>
@@ -2046,6 +2043,12 @@
   </si>
   <si>
     <t>ARRIVA\subchefcun</t>
+  </si>
+  <si>
+    <t>Areas Publicas</t>
+  </si>
+  <si>
+    <t>ARRIVA\apublicascun</t>
   </si>
 </sst>
 </file>
@@ -2707,9 +2710,9 @@
   <dimension ref="A1:X104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomLeft" activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2784,22 +2787,22 @@
         <v>11</v>
       </c>
       <c r="P1" s="7" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q1" s="7" t="s">
         <v>611</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="20" t="s">
         <v>612</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="S1" s="12" t="s">
         <v>613</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="T1" s="2" t="s">
         <v>614</v>
       </c>
-      <c r="T1" s="2" t="s">
-        <v>615</v>
-      </c>
       <c r="U1" s="7" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -2813,7 +2816,7 @@
         <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>23</v>
@@ -2829,7 +2832,7 @@
       </c>
       <c r="J2" s="3"/>
       <c r="L2" s="3" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>27</v>
@@ -2838,13 +2841,13 @@
         <v>20</v>
       </c>
       <c r="P2" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>620</v>
-      </c>
       <c r="R2" s="16" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="S2" s="13">
         <v>44829</v>
@@ -2853,7 +2856,7 @@
         <v>45194</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -2867,7 +2870,7 @@
         <v>25</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>23</v>
@@ -2883,7 +2886,7 @@
       </c>
       <c r="J3" s="3"/>
       <c r="L3" s="3" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>27</v>
@@ -2892,13 +2895,13 @@
         <v>20</v>
       </c>
       <c r="P3" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="Q3" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>620</v>
-      </c>
       <c r="R3" s="17" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="S3" s="13">
         <v>45563</v>
@@ -2907,7 +2910,7 @@
         <v>45563</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -2921,7 +2924,7 @@
         <v>436</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>14</v>
@@ -2936,7 +2939,7 @@
         <v>219</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>310</v>
@@ -2951,13 +2954,13 @@
         <v>141</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R4" s="17" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="S4" s="13">
         <v>45513</v>
@@ -2966,7 +2969,7 @@
         <v>46607</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -2977,10 +2980,10 @@
         <v>46</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>14</v>
@@ -2995,7 +2998,7 @@
         <v>220</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>310</v>
@@ -3010,13 +3013,13 @@
         <v>142</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="S5" s="13">
         <v>44781</v>
@@ -3025,7 +3028,7 @@
         <v>45876</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -3033,10 +3036,10 @@
         <v>47</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>14</v>
@@ -3052,7 +3055,7 @@
       </c>
       <c r="I6" s="21"/>
       <c r="J6" s="3" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>310</v>
@@ -3067,13 +3070,13 @@
         <v>143</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R6" s="17" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="S6" s="13">
         <v>44772</v>
@@ -3082,7 +3085,7 @@
         <v>45867</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -3093,10 +3096,10 @@
         <v>49</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>14</v>
@@ -3111,7 +3114,7 @@
         <v>223</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>310</v>
@@ -3126,13 +3129,13 @@
         <v>145</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R7" s="17" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="S7" s="13">
         <v>44441</v>
@@ -3141,7 +3144,7 @@
         <v>45537</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -3152,7 +3155,7 @@
         <v>438</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>14</v>
@@ -3167,7 +3170,7 @@
         <v>224</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>310</v>
@@ -3182,13 +3185,13 @@
         <v>146</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="R8" s="17" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="S8" s="13">
         <v>45468</v>
@@ -3197,7 +3200,7 @@
         <v>46562</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -3211,7 +3214,7 @@
         <v>439</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>14</v>
@@ -3226,7 +3229,7 @@
         <v>225</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>311</v>
@@ -3245,7 +3248,7 @@
         <v>46149</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -3256,10 +3259,10 @@
         <v>52</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>14</v>
@@ -3274,7 +3277,7 @@
         <v>226</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>311</v>
@@ -3289,13 +3292,13 @@
         <v>147</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="R10" s="17" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="S10" s="13">
         <v>45119</v>
@@ -3304,7 +3307,7 @@
         <v>46214</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -3315,10 +3318,10 @@
         <v>54</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>14</v>
@@ -3333,7 +3336,7 @@
         <v>228</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>311</v>
@@ -3348,13 +3351,13 @@
         <v>149</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R11" s="17" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="S11" s="13">
         <v>45016</v>
@@ -3363,7 +3366,7 @@
         <v>46111</v>
       </c>
       <c r="U11" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -3377,7 +3380,7 @@
         <v>444</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>14</v>
@@ -3392,7 +3395,7 @@
         <v>232</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>314</v>
@@ -3407,7 +3410,7 @@
         <v>152</v>
       </c>
       <c r="R12" s="17" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="S12" s="13">
         <v>44707</v>
@@ -3416,7 +3419,7 @@
         <v>45802</v>
       </c>
       <c r="U12" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -3430,7 +3433,7 @@
         <v>445</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>14</v>
@@ -3445,7 +3448,7 @@
         <v>233</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>314</v>
@@ -3460,13 +3463,13 @@
         <v>153</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R13" s="17" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="S13" s="13">
         <v>45012</v>
@@ -3475,7 +3478,7 @@
         <v>46107</v>
       </c>
       <c r="U13" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -3489,7 +3492,7 @@
         <v>448</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>14</v>
@@ -3504,7 +3507,7 @@
         <v>237</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>314</v>
@@ -3519,13 +3522,13 @@
         <v>155</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R14" s="17" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="S14" s="13">
         <v>44833</v>
@@ -3534,7 +3537,7 @@
         <v>45928</v>
       </c>
       <c r="U14" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -3548,7 +3551,7 @@
         <v>427</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>14</v>
@@ -3578,13 +3581,13 @@
         <v>21</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R15" s="17" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="S15" s="13">
         <v>45498</v>
@@ -3593,7 +3596,7 @@
         <v>46595</v>
       </c>
       <c r="U15" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -3607,7 +3610,7 @@
         <v>428</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>14</v>
@@ -3637,13 +3640,13 @@
         <v>134</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R16" s="17" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="S16" s="13">
         <v>44442</v>
@@ -3652,7 +3655,7 @@
         <v>45537</v>
       </c>
       <c r="U16" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -3666,7 +3669,7 @@
         <v>429</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>14</v>
@@ -3696,13 +3699,13 @@
         <v>135</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R17" s="17" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="S17" s="13">
         <v>45498</v>
@@ -3711,7 +3714,7 @@
         <v>46592</v>
       </c>
       <c r="U17" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -3725,7 +3728,7 @@
         <v>453</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>14</v>
@@ -3740,7 +3743,7 @@
         <v>243</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>316</v>
@@ -3755,13 +3758,13 @@
         <v>161</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R18" s="17" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="S18" s="13">
         <v>44439</v>
@@ -3770,7 +3773,7 @@
         <v>45534</v>
       </c>
       <c r="U18" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -3784,7 +3787,7 @@
         <v>453</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>14</v>
@@ -3799,7 +3802,7 @@
         <v>244</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>316</v>
@@ -3814,13 +3817,13 @@
         <v>162</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R19" s="17" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="S19" s="13">
         <v>45020</v>
@@ -3829,7 +3832,7 @@
         <v>46115</v>
       </c>
       <c r="U19" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -3843,7 +3846,7 @@
         <v>443</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>14</v>
@@ -3858,7 +3861,7 @@
         <v>245</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>316</v>
@@ -3873,13 +3876,13 @@
         <v>163</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R20" s="17" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="S20" s="13">
         <v>45020</v>
@@ -3888,7 +3891,7 @@
         <v>46115</v>
       </c>
       <c r="U20" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -3899,10 +3902,10 @@
         <v>73</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>14</v>
@@ -3917,7 +3920,7 @@
         <v>247</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>317</v>
@@ -3932,13 +3935,13 @@
         <v>164</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q21" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R21" s="17" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="S21" s="13">
         <v>44701</v>
@@ -3947,7 +3950,7 @@
         <v>45796</v>
       </c>
       <c r="U21" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="22" spans="1:21">
@@ -3958,7 +3961,7 @@
         <v>454</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>14</v>
@@ -3973,7 +3976,7 @@
         <v>248</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>317</v>
@@ -3988,13 +3991,13 @@
         <v>165</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R22" s="17" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="S22" s="13">
         <v>44657</v>
@@ -4003,7 +4006,7 @@
         <v>45752</v>
       </c>
       <c r="U22" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -4015,7 +4018,7 @@
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>14</v>
@@ -4041,7 +4044,7 @@
       </c>
       <c r="O23"/>
       <c r="R23" s="17" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="S23" s="13">
         <v>43580</v>
@@ -4050,7 +4053,7 @@
         <v>44700</v>
       </c>
       <c r="U23" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -4061,10 +4064,10 @@
         <v>78</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>14</v>
@@ -4079,7 +4082,7 @@
         <v>252</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>317</v>
@@ -4094,13 +4097,13 @@
         <v>167</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R24" s="17" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="S24" s="13">
         <v>45849</v>
@@ -4109,7 +4112,7 @@
         <v>46944</v>
       </c>
       <c r="U24" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -4121,7 +4124,7 @@
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>14</v>
@@ -4136,7 +4139,7 @@
         <v>253</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="L25" s="3" t="s">
         <v>317</v>
@@ -4151,13 +4154,13 @@
         <v>168</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R25" s="17" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="S25" s="13">
         <v>44446</v>
@@ -4166,7 +4169,7 @@
         <v>45541</v>
       </c>
       <c r="U25" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="26" spans="1:21">
@@ -4180,7 +4183,7 @@
         <v>457</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>14</v>
@@ -4195,7 +4198,7 @@
         <v>254</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>317</v>
@@ -4210,13 +4213,13 @@
         <v>169</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q26" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R26" s="17" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="S26" s="13">
         <v>45012</v>
@@ -4225,7 +4228,7 @@
         <v>46107</v>
       </c>
       <c r="U26" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="27" spans="1:21">
@@ -4239,7 +4242,7 @@
         <v>461</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>14</v>
@@ -4254,7 +4257,7 @@
         <v>258</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="L27" s="3" t="s">
         <v>317</v>
@@ -4269,13 +4272,13 @@
         <v>173</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q27" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R27" s="17" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="S27" s="13">
         <v>44664</v>
@@ -4284,7 +4287,7 @@
         <v>45759</v>
       </c>
       <c r="U27" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="28" spans="1:21">
@@ -4298,7 +4301,7 @@
         <v>462</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>14</v>
@@ -4313,7 +4316,7 @@
         <v>259</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="L28" s="3" t="s">
         <v>317</v>
@@ -4328,13 +4331,13 @@
         <v>174</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q28" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R28" s="19" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="S28" s="13">
         <v>45386</v>
@@ -4343,7 +4346,7 @@
         <v>46115</v>
       </c>
       <c r="U28" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="29" spans="1:21">
@@ -4357,7 +4360,7 @@
         <v>469</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>14</v>
@@ -4372,7 +4375,7 @@
         <v>266</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="L29" s="3" t="s">
         <v>317</v>
@@ -4387,13 +4390,13 @@
         <v>181</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q29" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R29" s="17" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="S29" s="13">
         <v>44377</v>
@@ -4402,7 +4405,7 @@
         <v>45472</v>
       </c>
       <c r="U29" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="30" spans="1:21">
@@ -4413,7 +4416,7 @@
         <v>480</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>14</v>
@@ -4428,7 +4431,7 @@
         <v>282</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="L30" s="3" t="s">
         <v>26</v>
@@ -4443,13 +4446,13 @@
         <v>195</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q30" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R30" s="15" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="S30" s="13">
         <v>45894</v>
@@ -4458,7 +4461,7 @@
         <v>46989</v>
       </c>
       <c r="U30" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="31" spans="1:21">
@@ -4472,7 +4475,7 @@
         <v>430</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>14</v>
@@ -4487,7 +4490,7 @@
         <v>214</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="L31" s="3" t="s">
         <v>309</v>
@@ -4502,13 +4505,13 @@
         <v>136</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="R31" s="17" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="S31" s="13">
         <v>45498</v>
@@ -4517,7 +4520,7 @@
         <v>46592</v>
       </c>
       <c r="U31" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="32" spans="1:21">
@@ -4528,7 +4531,7 @@
         <v>431</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>14</v>
@@ -4558,13 +4561,13 @@
         <v>137</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q32" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R32" s="17" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="S32" s="13">
         <v>45498</v>
@@ -4573,7 +4576,7 @@
         <v>46592</v>
       </c>
       <c r="U32" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="33" spans="1:21">
@@ -4587,7 +4590,7 @@
         <v>432</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>14</v>
@@ -4602,7 +4605,7 @@
         <v>216</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="L33" s="3" t="s">
         <v>309</v>
@@ -4617,13 +4620,13 @@
         <v>138</v>
       </c>
       <c r="P33" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q33" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R33" s="17" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="S33" s="13">
         <v>45519</v>
@@ -4632,7 +4635,7 @@
         <v>46613</v>
       </c>
       <c r="U33" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="34" spans="1:21">
@@ -4646,7 +4649,7 @@
         <v>433</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>14</v>
@@ -4661,10 +4664,10 @@
         <v>217</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>502</v>
+        <v>669</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>309</v>
+        <v>668</v>
       </c>
       <c r="M34" s="3" t="s">
         <v>319</v>
@@ -4676,13 +4679,13 @@
         <v>139</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q34" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R34" s="17" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="S34" s="13">
         <v>45849</v>
@@ -4691,7 +4694,7 @@
         <v>46944</v>
       </c>
       <c r="U34" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="35" spans="1:21">
@@ -4705,7 +4708,7 @@
         <v>449</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>14</v>
@@ -4720,7 +4723,7 @@
         <v>238</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="L35" s="3" t="s">
         <v>315</v>
@@ -4735,13 +4738,13 @@
         <v>156</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="Q35" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="R35" s="18" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="S35" s="13">
         <v>45021</v>
@@ -4750,7 +4753,7 @@
         <v>46116</v>
       </c>
       <c r="U35" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="36" spans="1:21">
@@ -4764,7 +4767,7 @@
         <v>450</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>14</v>
@@ -4779,7 +4782,7 @@
         <v>239</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L36" s="3" t="s">
         <v>315</v>
@@ -4794,13 +4797,13 @@
         <v>157</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="Q36" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="R36" s="17" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="S36" s="13">
         <v>45883</v>
@@ -4809,7 +4812,7 @@
         <v>46978</v>
       </c>
       <c r="U36" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="37" spans="1:21">
@@ -4817,10 +4820,10 @@
         <v>66</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>14</v>
@@ -4835,7 +4838,7 @@
         <v>240</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L37" s="3" t="s">
         <v>315</v>
@@ -4850,13 +4853,13 @@
         <v>158</v>
       </c>
       <c r="P37" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="Q37" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="R37" s="17" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="S37" s="13">
         <v>44453</v>
@@ -4865,7 +4868,7 @@
         <v>44817</v>
       </c>
       <c r="U37" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="38" spans="1:21">
@@ -4879,7 +4882,7 @@
         <v>451</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>14</v>
@@ -4894,7 +4897,7 @@
         <v>241</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>315</v>
@@ -4909,13 +4912,13 @@
         <v>159</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q38" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R38" s="17" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="S38" s="13">
         <v>43605</v>
@@ -4924,7 +4927,7 @@
         <v>44700</v>
       </c>
       <c r="U38" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="39" spans="1:21">
@@ -4938,7 +4941,7 @@
         <v>452</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>14</v>
@@ -4953,7 +4956,7 @@
         <v>242</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>315</v>
@@ -4968,13 +4971,13 @@
         <v>160</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q39" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R39" s="17" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="S39" s="13">
         <v>45099</v>
@@ -4983,7 +4986,7 @@
         <v>46194</v>
       </c>
       <c r="U39" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="40" spans="1:21">
@@ -4997,7 +5000,7 @@
         <v>463</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>14</v>
@@ -5012,7 +5015,7 @@
         <v>260</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="L40" s="3" t="s">
         <v>322</v>
@@ -5027,13 +5030,13 @@
         <v>175</v>
       </c>
       <c r="P40" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q40" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R40" s="17" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="S40" s="13">
         <v>44183</v>
@@ -5042,7 +5045,7 @@
         <v>45277</v>
       </c>
       <c r="U40" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="41" spans="1:21">
@@ -5056,7 +5059,7 @@
         <v>475</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>14</v>
@@ -5071,7 +5074,7 @@
         <v>267</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="L41" s="3" t="s">
         <v>324</v>
@@ -5086,13 +5089,13 @@
         <v>182</v>
       </c>
       <c r="P41" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q41" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R41" s="17" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="S41" s="13">
         <v>44189</v>
@@ -5101,7 +5104,7 @@
         <v>45283</v>
       </c>
       <c r="U41" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="42" spans="1:21">
@@ -5115,7 +5118,7 @@
         <v>473</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>14</v>
@@ -5130,7 +5133,7 @@
         <v>268</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="L42" s="3" t="s">
         <v>324</v>
@@ -5145,13 +5148,13 @@
         <v>183</v>
       </c>
       <c r="P42" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q42" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R42" s="18" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="S42" s="13">
         <v>45849</v>
@@ -5160,7 +5163,7 @@
         <v>46944</v>
       </c>
       <c r="U42" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="43" spans="1:21">
@@ -5174,7 +5177,7 @@
         <v>474</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>14</v>
@@ -5189,7 +5192,7 @@
         <v>269</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="L43" s="3" t="s">
         <v>324</v>
@@ -5204,13 +5207,13 @@
         <v>184</v>
       </c>
       <c r="P43" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q43" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R43" s="17" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="S43" s="13">
         <v>45958</v>
@@ -5219,7 +5222,7 @@
         <v>47053</v>
       </c>
       <c r="U43" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="44" spans="1:21">
@@ -5233,7 +5236,7 @@
         <v>472</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>14</v>
@@ -5248,7 +5251,7 @@
         <v>270</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="L44" s="3" t="s">
         <v>324</v>
@@ -5263,13 +5266,13 @@
         <v>185</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q44" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R44" s="17" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="S44" s="13">
         <v>43580</v>
@@ -5278,7 +5281,7 @@
         <v>44700</v>
       </c>
       <c r="U44" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="45" spans="1:21">
@@ -5292,7 +5295,7 @@
         <v>471</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>14</v>
@@ -5307,7 +5310,7 @@
         <v>271</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="L45" s="3" t="s">
         <v>324</v>
@@ -5322,13 +5325,13 @@
         <v>186</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q45" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R45" s="17" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="S45" s="13">
         <v>45849</v>
@@ -5337,7 +5340,7 @@
         <v>46944</v>
       </c>
       <c r="U45" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="46" spans="1:21">
@@ -5351,7 +5354,7 @@
         <v>470</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>14</v>
@@ -5366,7 +5369,7 @@
         <v>272</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="L46" s="3" t="s">
         <v>324</v>
@@ -5381,13 +5384,13 @@
         <v>187</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q46" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R46" s="17" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="S46" s="13">
         <v>45012</v>
@@ -5396,7 +5399,7 @@
         <v>46107</v>
       </c>
       <c r="U46" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="47" spans="1:21">
@@ -5410,7 +5413,7 @@
         <v>476</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>14</v>
@@ -5425,7 +5428,7 @@
         <v>273</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="L47" s="3" t="s">
         <v>324</v>
@@ -5440,13 +5443,13 @@
         <v>188</v>
       </c>
       <c r="P47" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q47" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R47" s="17" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="S47" s="13">
         <v>45537</v>
@@ -5455,7 +5458,7 @@
         <v>46631</v>
       </c>
       <c r="U47" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="48" spans="1:21">
@@ -5463,10 +5466,10 @@
         <v>104</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>14</v>
@@ -5494,10 +5497,10 @@
         <v>192</v>
       </c>
       <c r="P48" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q48" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="S48" s="13">
         <v>45146</v>
@@ -5506,7 +5509,7 @@
         <v>46256</v>
       </c>
       <c r="U48" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="49" spans="1:21">
@@ -5514,10 +5517,10 @@
         <v>107</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>14</v>
@@ -5527,7 +5530,7 @@
       </c>
       <c r="H49" s="1"/>
       <c r="J49" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="L49" s="3" t="s">
         <v>326</v>
@@ -5542,7 +5545,7 @@
         <v>193</v>
       </c>
       <c r="U49" s="3" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="50" spans="1:21">
@@ -5550,10 +5553,10 @@
         <v>108</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>14</v>
@@ -5568,7 +5571,7 @@
         <v>280</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="L50" s="3" t="s">
         <v>326</v>
@@ -5589,7 +5592,7 @@
         <v>46607</v>
       </c>
       <c r="U50" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="51" spans="1:21">
@@ -5600,7 +5603,7 @@
         <v>479</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>14</v>
@@ -5615,7 +5618,7 @@
         <v>281</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="L51" s="3" t="s">
         <v>326</v>
@@ -5627,16 +5630,16 @@
         <v>20</v>
       </c>
       <c r="O51" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="P51" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q51" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R51" s="15" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="S51" s="13">
         <v>44699</v>
@@ -5645,7 +5648,7 @@
         <v>45794</v>
       </c>
       <c r="U51" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="52" spans="1:21">
@@ -5659,7 +5662,7 @@
         <v>486</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>14</v>
@@ -5674,7 +5677,7 @@
         <v>291</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="L52" s="3" t="s">
         <v>315</v>
@@ -5689,13 +5692,13 @@
         <v>201</v>
       </c>
       <c r="P52" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="Q52" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="R52" s="17" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="S52" s="13">
         <v>43580</v>
@@ -5704,7 +5707,7 @@
         <v>44700</v>
       </c>
       <c r="U52" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="53" spans="1:21">
@@ -5718,7 +5721,7 @@
         <v>487</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>14</v>
@@ -5733,7 +5736,7 @@
         <v>292</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="L53" s="3" t="s">
         <v>328</v>
@@ -5748,10 +5751,10 @@
         <v>202</v>
       </c>
       <c r="P53" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="Q53" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="S53" s="13">
         <v>43108</v>
@@ -5760,7 +5763,7 @@
         <v>43564</v>
       </c>
       <c r="U53" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="54" spans="1:21">
@@ -5768,10 +5771,10 @@
         <v>124</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>14</v>
@@ -5786,7 +5789,7 @@
         <v>296</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="L54" s="3" t="s">
         <v>321</v>
@@ -5801,13 +5804,13 @@
         <v>204</v>
       </c>
       <c r="P54" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q54" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R54" s="17" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="S54" s="13">
         <v>45112</v>
@@ -5816,7 +5819,7 @@
         <v>46207</v>
       </c>
       <c r="U54" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="55" spans="1:21">
@@ -5827,7 +5830,7 @@
         <v>492</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>14</v>
@@ -5842,7 +5845,7 @@
         <v>299</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L55" s="3" t="s">
         <v>321</v>
@@ -5855,13 +5858,13 @@
       </c>
       <c r="O55"/>
       <c r="P55" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="Q55" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="R55" s="17" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="S55" s="13">
         <v>44697</v>
@@ -5870,7 +5873,7 @@
         <v>45792</v>
       </c>
       <c r="U55" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="56" spans="1:21">
@@ -5878,10 +5881,10 @@
         <v>128</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>14</v>
@@ -5896,7 +5899,7 @@
         <v>300</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="L56" s="3" t="s">
         <v>321</v>
@@ -5911,13 +5914,13 @@
         <v>207</v>
       </c>
       <c r="P56" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q56" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R56" s="17" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="S56" s="13">
         <v>45349</v>
@@ -5926,7 +5929,7 @@
         <v>46444</v>
       </c>
       <c r="U56" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="57" spans="1:21">
@@ -5934,10 +5937,10 @@
         <v>129</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>14</v>
@@ -5946,13 +5949,13 @@
         <v>305</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>301</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="L57" s="3" t="s">
         <v>321</v>
@@ -5971,7 +5974,7 @@
         <v>43598</v>
       </c>
       <c r="U57" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="58" spans="1:21">
@@ -5982,7 +5985,7 @@
         <v>493</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>14</v>
@@ -5997,7 +6000,7 @@
         <v>303</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="L58" s="3" t="s">
         <v>321</v>
@@ -6012,10 +6015,10 @@
         <v>209</v>
       </c>
       <c r="P58" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q58" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="S58" s="13">
         <v>43066</v>
@@ -6024,7 +6027,7 @@
         <v>43522</v>
       </c>
       <c r="U58" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="59" spans="1:21">
@@ -6038,7 +6041,7 @@
         <v>464</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>14</v>
@@ -6053,7 +6056,7 @@
         <v>261</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="L59" s="3" t="s">
         <v>323</v>
@@ -6068,13 +6071,13 @@
         <v>176</v>
       </c>
       <c r="P59" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q59" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R59" s="19" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="S59" s="13">
         <v>44699</v>
@@ -6083,7 +6086,7 @@
         <v>45794</v>
       </c>
       <c r="U59" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="60" spans="1:21">
@@ -6097,7 +6100,7 @@
         <v>465</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>14</v>
@@ -6112,7 +6115,7 @@
         <v>262</v>
       </c>
       <c r="J60" s="9" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="L60" s="3" t="s">
         <v>323</v>
@@ -6127,13 +6130,13 @@
         <v>177</v>
       </c>
       <c r="P60" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q60" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R60" s="19" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="S60" s="13">
         <v>45118</v>
@@ -6142,7 +6145,7 @@
         <v>46213</v>
       </c>
       <c r="U60" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="61" spans="1:21">
@@ -6156,7 +6159,7 @@
         <v>466</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>14</v>
@@ -6171,7 +6174,7 @@
         <v>263</v>
       </c>
       <c r="J61" s="9" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="L61" s="3" t="s">
         <v>323</v>
@@ -6186,13 +6189,13 @@
         <v>178</v>
       </c>
       <c r="P61" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q61" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R61" s="19" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="S61" s="13">
         <v>45099</v>
@@ -6201,7 +6204,7 @@
         <v>46194</v>
       </c>
       <c r="U61" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="62" spans="1:21">
@@ -6215,7 +6218,7 @@
         <v>468</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>14</v>
@@ -6230,7 +6233,7 @@
         <v>265</v>
       </c>
       <c r="J62" s="9" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="L62" s="3" t="s">
         <v>323</v>
@@ -6245,13 +6248,13 @@
         <v>180</v>
       </c>
       <c r="P62" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q62" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R62" s="17" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="S62" s="13">
         <v>44664</v>
@@ -6260,7 +6263,7 @@
         <v>45759</v>
       </c>
       <c r="U62" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="63" spans="1:21">
@@ -6274,7 +6277,7 @@
         <v>482</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>14</v>
@@ -6289,7 +6292,7 @@
         <v>286</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="L63" s="3" t="s">
         <v>327</v>
@@ -6304,13 +6307,13 @@
         <v>197</v>
       </c>
       <c r="P63" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q63" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R63" s="15" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="S63" s="13">
         <v>45264</v>
@@ -6319,7 +6322,7 @@
         <v>46359</v>
       </c>
       <c r="U63" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="64" spans="1:21">
@@ -6333,7 +6336,7 @@
         <v>483</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>14</v>
@@ -6348,7 +6351,7 @@
         <v>287</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="L64" s="3" t="s">
         <v>327</v>
@@ -6363,13 +6366,13 @@
         <v>198</v>
       </c>
       <c r="P64" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q64" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R64" s="17" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="S64" s="13">
         <v>45264</v>
@@ -6378,7 +6381,7 @@
         <v>46389</v>
       </c>
       <c r="U64" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="65" spans="1:21">
@@ -6392,7 +6395,7 @@
         <v>434</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>14</v>
@@ -6420,13 +6423,13 @@
         <v>140</v>
       </c>
       <c r="P65" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="Q65" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="R65" s="17" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="S65" s="13">
         <v>45895</v>
@@ -6435,7 +6438,7 @@
         <v>46990</v>
       </c>
       <c r="U65" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="66" spans="1:21">
@@ -6449,7 +6452,7 @@
         <v>477</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>14</v>
@@ -6464,7 +6467,7 @@
         <v>274</v>
       </c>
       <c r="J66" s="9" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L66" s="3" t="s">
         <v>325</v>
@@ -6479,13 +6482,13 @@
         <v>189</v>
       </c>
       <c r="P66" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="Q66" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="R66" s="17" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="S66" s="13">
         <v>45539</v>
@@ -6494,7 +6497,7 @@
         <v>46633</v>
       </c>
       <c r="U66" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="67" spans="1:21">
@@ -6508,7 +6511,7 @@
         <v>477</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>14</v>
@@ -6523,7 +6526,7 @@
         <v>275</v>
       </c>
       <c r="J67" s="9" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="L67" s="3" t="s">
         <v>325</v>
@@ -6538,13 +6541,13 @@
         <v>190</v>
       </c>
       <c r="P67" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="Q67" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="R67" s="17" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="S67" s="13">
         <v>45547</v>
@@ -6553,7 +6556,7 @@
         <v>46641</v>
       </c>
       <c r="U67" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="68" spans="1:21">
@@ -6567,7 +6570,7 @@
         <v>488</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>14</v>
@@ -6582,7 +6585,7 @@
         <v>293</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="L68" s="3" t="s">
         <v>312</v>
@@ -6597,13 +6600,13 @@
         <v>203</v>
       </c>
       <c r="P68" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="Q68" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="R68" s="17" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="S68" s="13">
         <v>45498</v>
@@ -6612,7 +6615,7 @@
         <v>46592</v>
       </c>
       <c r="U68" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="69" spans="1:21">
@@ -6626,7 +6629,7 @@
         <v>437</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>133</v>
@@ -6641,7 +6644,7 @@
         <v>222</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L69" s="3" t="s">
         <v>310</v>
@@ -6656,13 +6659,13 @@
         <v>144</v>
       </c>
       <c r="P69" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q69" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R69" s="17" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="S69" s="13">
         <v>45516</v>
@@ -6671,7 +6674,7 @@
         <v>46610</v>
       </c>
       <c r="U69" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="70" spans="1:21">
@@ -6682,10 +6685,10 @@
         <v>53</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>133</v>
@@ -6700,7 +6703,7 @@
         <v>227</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="L70" s="3" t="s">
         <v>311</v>
@@ -6715,13 +6718,13 @@
         <v>148</v>
       </c>
       <c r="P70" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="Q70" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="Q70" s="3" t="s">
-        <v>620</v>
-      </c>
       <c r="R70" s="17" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="S70" s="13">
         <v>45026</v>
@@ -6730,7 +6733,7 @@
         <v>46121</v>
       </c>
       <c r="U70" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="71" spans="1:21">
@@ -6741,7 +6744,7 @@
         <v>440</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>133</v>
@@ -6756,7 +6759,7 @@
         <v>229</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="L71" s="3" t="s">
         <v>311</v>
@@ -6771,13 +6774,13 @@
         <v>150</v>
       </c>
       <c r="P71" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q71" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R71" s="17" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="S71" s="13">
         <v>44716</v>
@@ -6786,7 +6789,7 @@
         <v>45811</v>
       </c>
       <c r="U71" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="72" spans="1:21">
@@ -6800,7 +6803,7 @@
         <v>446</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>133</v>
@@ -6815,7 +6818,7 @@
         <v>234</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L72" s="3" t="s">
         <v>314</v>
@@ -6830,13 +6833,13 @@
         <v>154</v>
       </c>
       <c r="P72" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q72" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R72" s="17" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="S72" s="13">
         <v>44667</v>
@@ -6845,7 +6848,7 @@
         <v>45762</v>
       </c>
       <c r="U72" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="73" spans="1:21">
@@ -6856,10 +6859,10 @@
         <v>61</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>133</v>
@@ -6874,7 +6877,7 @@
         <v>235</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L73" s="3" t="s">
         <v>314</v>
@@ -6887,13 +6890,13 @@
       </c>
       <c r="O73"/>
       <c r="P73" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q73" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R73" s="17" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="S73" s="13">
         <v>45517</v>
@@ -6902,7 +6905,7 @@
         <v>46611</v>
       </c>
       <c r="U73" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="74" spans="1:21">
@@ -6916,7 +6919,7 @@
         <v>447</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>133</v>
@@ -6931,7 +6934,7 @@
         <v>236</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="L74" s="3" t="s">
         <v>314</v>
@@ -6943,16 +6946,16 @@
         <v>20</v>
       </c>
       <c r="O74" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="P74" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q74" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R74" s="17" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="S74" s="13">
         <v>45873</v>
@@ -6961,7 +6964,7 @@
         <v>46968</v>
       </c>
       <c r="U74" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="75" spans="1:21">
@@ -6970,7 +6973,7 @@
       </c>
       <c r="C75" s="4"/>
       <c r="D75" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>133</v>
@@ -6998,10 +7001,10 @@
         <v>421</v>
       </c>
       <c r="P75" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q75" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="S75" s="13">
         <v>43526</v>
@@ -7010,7 +7013,7 @@
         <v>44641</v>
       </c>
       <c r="U75" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="76" spans="1:21">
@@ -7024,7 +7027,7 @@
         <v>442</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>133</v>
@@ -7039,7 +7042,7 @@
         <v>231</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="L76" s="3" t="s">
         <v>313</v>
@@ -7054,13 +7057,13 @@
         <v>151</v>
       </c>
       <c r="P76" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q76" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R76" s="17" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="S76" s="13">
         <v>45762</v>
@@ -7069,7 +7072,7 @@
         <v>46857</v>
       </c>
       <c r="U76" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="77" spans="1:21">
@@ -7077,10 +7080,10 @@
         <v>72</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>133</v>
@@ -7095,7 +7098,7 @@
         <v>246</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="L77" s="3" t="s">
         <v>317</v>
@@ -7108,13 +7111,13 @@
       </c>
       <c r="O77"/>
       <c r="P77" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q77" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R77" s="17" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="S77" s="13">
         <v>45058</v>
@@ -7123,7 +7126,7 @@
         <v>46153</v>
       </c>
       <c r="U77" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="78" spans="1:21">
@@ -7137,7 +7140,7 @@
         <v>495</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>133</v>
@@ -7152,7 +7155,7 @@
         <v>339</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L78" s="3" t="s">
         <v>317</v>
@@ -7167,13 +7170,13 @@
         <v>340</v>
       </c>
       <c r="P78" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q78" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R78" s="17" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="S78" s="13">
         <v>45514</v>
@@ -7182,7 +7185,7 @@
         <v>46608</v>
       </c>
       <c r="U78" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="79" spans="1:21">
@@ -7196,7 +7199,7 @@
         <v>455</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>133</v>
@@ -7211,7 +7214,7 @@
         <v>250</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L79" s="3" t="s">
         <v>210</v>
@@ -7223,16 +7226,16 @@
         <v>20</v>
       </c>
       <c r="O79" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="P79" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q79" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R79" s="17" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="S79" s="13">
         <v>45856</v>
@@ -7241,7 +7244,7 @@
         <v>46951</v>
       </c>
       <c r="U79" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="80" spans="1:21">
@@ -7255,7 +7258,7 @@
         <v>456</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>133</v>
@@ -7270,7 +7273,7 @@
         <v>251</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L80" s="3" t="s">
         <v>318</v>
@@ -7285,13 +7288,13 @@
         <v>166</v>
       </c>
       <c r="P80" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q80" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R80" s="17" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="S80" s="13">
         <v>45518</v>
@@ -7300,7 +7303,7 @@
         <v>46612</v>
       </c>
       <c r="U80" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="81" spans="1:23">
@@ -7311,7 +7314,7 @@
         <v>480</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>133</v>
@@ -7326,7 +7329,7 @@
         <v>283</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="L81" s="3" t="s">
         <v>26</v>
@@ -7339,22 +7342,22 @@
       </c>
       <c r="O81"/>
       <c r="P81" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q81" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R81" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="S81" s="13">
         <v>43755</v>
       </c>
       <c r="T81" s="3" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="U81" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="82" spans="1:23">
@@ -7368,7 +7371,7 @@
         <v>481</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>133</v>
@@ -7383,7 +7386,7 @@
         <v>284</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="L82" s="3" t="s">
         <v>26</v>
@@ -7395,16 +7398,16 @@
         <v>20</v>
       </c>
       <c r="O82" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="P82" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q82" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R82" s="15" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="S82" s="13">
         <v>45513</v>
@@ -7413,7 +7416,7 @@
         <v>46607</v>
       </c>
       <c r="U82" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="83" spans="1:23">
@@ -7427,7 +7430,7 @@
         <v>458</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>133</v>
@@ -7439,10 +7442,10 @@
         <v>352</v>
       </c>
       <c r="H83" s="14" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="L83" s="3" t="s">
         <v>319</v>
@@ -7457,13 +7460,13 @@
         <v>170</v>
       </c>
       <c r="P83" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q83" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R83" s="17" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="S83" s="13">
         <v>44664</v>
@@ -7472,7 +7475,7 @@
         <v>45759</v>
       </c>
       <c r="U83" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="84" spans="1:23">
@@ -7483,10 +7486,10 @@
         <v>105</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>133</v>
@@ -7501,7 +7504,7 @@
         <v>278</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="L84" s="3" t="s">
         <v>326</v>
@@ -7520,7 +7523,7 @@
         <v>46852</v>
       </c>
       <c r="U84" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="85" spans="1:23">
@@ -7528,10 +7531,10 @@
         <v>106</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>133</v>
@@ -7546,7 +7549,7 @@
         <v>279</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="L85" s="3" t="s">
         <v>326</v>
@@ -7559,7 +7562,7 @@
       </c>
       <c r="O85"/>
       <c r="R85" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="S85" s="13">
         <v>44425</v>
@@ -7568,7 +7571,7 @@
         <v>45520</v>
       </c>
       <c r="U85" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="86" spans="1:23">
@@ -7579,7 +7582,7 @@
         <v>326</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>133</v>
@@ -7594,7 +7597,7 @@
         <v>288</v>
       </c>
       <c r="J86" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="L86" s="3" t="s">
         <v>326</v>
@@ -7609,7 +7612,7 @@
         <v>199</v>
       </c>
       <c r="R86" s="17" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="S86" s="13">
         <v>45265</v>
@@ -7618,7 +7621,7 @@
         <v>46360</v>
       </c>
       <c r="U86" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="87" spans="1:23">
@@ -7632,7 +7635,7 @@
         <v>459</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>133</v>
@@ -7647,7 +7650,7 @@
         <v>255</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="L87" s="3" t="s">
         <v>320</v>
@@ -7662,13 +7665,13 @@
         <v>171</v>
       </c>
       <c r="P87" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q87" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R87" s="17" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="S87" s="13">
         <v>45848</v>
@@ -7677,7 +7680,7 @@
         <v>46943</v>
       </c>
       <c r="U87" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="88" spans="1:23">
@@ -7686,7 +7689,7 @@
       </c>
       <c r="C88" s="4"/>
       <c r="D88" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>133</v>
@@ -7701,7 +7704,7 @@
         <v>257</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="L88" s="3" t="s">
         <v>321</v>
@@ -7716,13 +7719,13 @@
         <v>172</v>
       </c>
       <c r="P88" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q88" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R88" s="17" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="S88" s="13">
         <v>45654</v>
@@ -7731,7 +7734,7 @@
         <v>46748</v>
       </c>
       <c r="U88" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="89" spans="1:23">
@@ -7740,7 +7743,7 @@
       </c>
       <c r="C89" s="4"/>
       <c r="D89" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>133</v>
@@ -7755,7 +7758,7 @@
         <v>295</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="L89" s="3" t="s">
         <v>321</v>
@@ -7767,16 +7770,16 @@
         <v>20</v>
       </c>
       <c r="O89" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="P89" s="11" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="Q89" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="R89" s="17" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="S89" s="13">
         <v>45419</v>
@@ -7785,7 +7788,7 @@
         <v>46513</v>
       </c>
       <c r="U89" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="W89" s="8"/>
     </row>
@@ -7797,7 +7800,7 @@
         <v>490</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>133</v>
@@ -7812,7 +7815,7 @@
         <v>297</v>
       </c>
       <c r="J90" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="L90" s="3" t="s">
         <v>321</v>
@@ -7827,13 +7830,13 @@
         <v>205</v>
       </c>
       <c r="P90" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q90" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R90" s="17" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="S90" s="13">
         <v>44697</v>
@@ -7842,7 +7845,7 @@
         <v>45792</v>
       </c>
       <c r="U90" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="91" spans="1:23">
@@ -7853,7 +7856,7 @@
         <v>491</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>133</v>
@@ -7868,7 +7871,7 @@
         <v>298</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="L91" s="3" t="s">
         <v>321</v>
@@ -7883,13 +7886,13 @@
         <v>206</v>
       </c>
       <c r="P91" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q91" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R91" s="17" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="S91" s="13">
         <v>44705</v>
@@ -7898,7 +7901,7 @@
         <v>45800</v>
       </c>
       <c r="U91" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="92" spans="1:23">
@@ -7906,10 +7909,10 @@
         <v>130</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>133</v>
@@ -7924,7 +7927,7 @@
         <v>302</v>
       </c>
       <c r="J92" s="3" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="L92" s="3" t="s">
         <v>321</v>
@@ -7939,10 +7942,10 @@
         <v>208</v>
       </c>
       <c r="P92" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="Q92" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="S92" s="13">
         <v>43427</v>
@@ -7951,7 +7954,7 @@
         <v>45272</v>
       </c>
       <c r="U92" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="93" spans="1:23">
@@ -7965,7 +7968,7 @@
         <v>467</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>133</v>
@@ -7980,7 +7983,7 @@
         <v>264</v>
       </c>
       <c r="J93" s="9" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="L93" s="3" t="s">
         <v>323</v>
@@ -7995,13 +7998,13 @@
         <v>179</v>
       </c>
       <c r="P93" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q93" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R93" s="17" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="S93" s="13">
         <v>45012</v>
@@ -8010,7 +8013,7 @@
         <v>46107</v>
       </c>
       <c r="U93" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="94" spans="1:23">
@@ -8024,7 +8027,7 @@
         <v>484</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>133</v>
@@ -8039,7 +8042,7 @@
         <v>289</v>
       </c>
       <c r="J94" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="L94" s="3" t="s">
         <v>327</v>
@@ -8051,16 +8054,16 @@
         <v>20</v>
       </c>
       <c r="O94" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="P94" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q94" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R94" s="17" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="S94" s="13">
         <v>45265</v>
@@ -8069,7 +8072,7 @@
         <v>46360</v>
       </c>
       <c r="U94" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="95" spans="1:23">
@@ -8080,7 +8083,7 @@
         <v>441</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>133</v>
@@ -8095,7 +8098,7 @@
         <v>230</v>
       </c>
       <c r="J95" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="L95" s="3" t="s">
         <v>312</v>
@@ -8107,16 +8110,16 @@
         <v>20</v>
       </c>
       <c r="O95" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="P95" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q95" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R95" s="17" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="S95" s="13">
         <v>45502</v>
@@ -8125,7 +8128,7 @@
         <v>46596</v>
       </c>
       <c r="U95" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="96" spans="1:23">
@@ -8139,7 +8142,7 @@
         <v>460</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>133</v>
@@ -8154,7 +8157,7 @@
         <v>256</v>
       </c>
       <c r="J96" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="L96" s="3" t="s">
         <v>312</v>
@@ -8166,16 +8169,16 @@
         <v>20</v>
       </c>
       <c r="O96" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="P96" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q96" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R96" s="17" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="S96" s="13">
         <v>45024</v>
@@ -8184,7 +8187,7 @@
         <v>46119</v>
       </c>
       <c r="U96" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="97" spans="1:24">
@@ -8198,7 +8201,7 @@
         <v>478</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>133</v>
@@ -8213,7 +8216,7 @@
         <v>276</v>
       </c>
       <c r="J97" s="9" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="L97" s="3" t="s">
         <v>325</v>
@@ -8228,13 +8231,13 @@
         <v>191</v>
       </c>
       <c r="P97" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q97" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R97" s="17" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="S97" s="13">
         <v>44980</v>
@@ -8243,7 +8246,7 @@
         <v>46075</v>
       </c>
       <c r="U97" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="98" spans="1:24">
@@ -8257,7 +8260,7 @@
         <v>211</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>133</v>
@@ -8272,7 +8275,7 @@
         <v>285</v>
       </c>
       <c r="J98" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="L98" s="3" t="s">
         <v>211</v>
@@ -8287,13 +8290,13 @@
         <v>196</v>
       </c>
       <c r="P98" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q98" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R98" s="15" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="S98" s="13">
         <v>45517</v>
@@ -8302,7 +8305,7 @@
         <v>46611</v>
       </c>
       <c r="U98" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="99" spans="1:24">
@@ -8313,7 +8316,7 @@
         <v>489</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>133</v>
@@ -8328,7 +8331,7 @@
         <v>294</v>
       </c>
       <c r="J99" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="L99" s="3" t="s">
         <v>312</v>
@@ -8340,16 +8343,16 @@
         <v>20</v>
       </c>
       <c r="O99" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="P99" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q99" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R99" s="17" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="S99" s="13">
         <v>44694</v>
@@ -8358,7 +8361,7 @@
         <v>45789</v>
       </c>
       <c r="U99" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="100" spans="1:24">
@@ -8369,7 +8372,7 @@
         <v>435</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>34</v>
@@ -8397,13 +8400,13 @@
         <v>37</v>
       </c>
       <c r="P100" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="Q100" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="U100" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="101" spans="1:24">
@@ -8414,7 +8417,7 @@
         <v>485</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>34</v>
@@ -8442,7 +8445,7 @@
         <v>200</v>
       </c>
       <c r="R101" s="17" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="S101" s="13">
         <v>45897</v>
@@ -8451,7 +8454,7 @@
         <v>46992</v>
       </c>
       <c r="U101" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="102" spans="1:24">
@@ -8462,7 +8465,7 @@
         <v>494</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>34</v>
@@ -8488,7 +8491,7 @@
       </c>
       <c r="O102"/>
       <c r="U102" s="3" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="103" spans="1:24">

</xml_diff>